<commit_message>
Added Igniter Sequence and update Request DAQ sequence
</commit_message>
<xml_diff>
--- a/requirements_design/HCS_Requirements_Documentation.xlsx
+++ b/requirements_design/HCS_Requirements_Documentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7975897b035f41c7/my_files/UVIC/ROCKETRY/UVicRocketry_GITHUB/Hybrid-Controls-System/requirements_design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="253" documentId="11_F25DC773A252ABDACC104806C9D97FB05ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{41689EEE-19B1-4C1B-B9A6-29B5B7FEC886}"/>
+  <xr:revisionPtr revIDLastSave="263" documentId="11_F25DC773A252ABDACC104806C9D97FB05ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E5AC490-5FE7-415D-AC4D-ED470D76A62C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="System" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="273">
   <si>
     <t>Date Changed</t>
   </si>
@@ -1103,6 +1103,44 @@
   </si>
   <si>
     <t>Created Initial Requirements</t>
+  </si>
+  <si>
+    <t>As a user, I want the test stand to respond to the instruction I command through the UI. (Given a working system, when I toggle the states of valve in the control UI, the valves change state on the test stand in accordance).</t>
+  </si>
+  <si>
+    <t>Entire System</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">As a user, I want to have the ability to initiate a abort sequence </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>at any time.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (Given a working system, when I notice a dangerous event occuring at the test stand, I can quickly initiate a shutdown procedure).</t>
+    </r>
+  </si>
+  <si>
+    <t>As a user, I want to control the test stand from a safe distance.</t>
+  </si>
+  <si>
+    <t>As a user, I want the system to respond to my input as close to realtime as possible (especially when considering the ABORT command). (Given</t>
   </si>
 </sst>
 </file>
@@ -1197,10 +1235,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="9">
@@ -1390,24 +1430,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="20"/>
-        <color theme="7"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1473,6 +1495,31 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thick">
+          <color theme="4"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color theme="7"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -1523,13 +1570,6 @@
         <family val="2"/>
       </font>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thick">
-          <color theme="4"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1659,37 +1699,37 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{F8107C66-607B-4058-88D5-7E54DAB777F3}" name="Table112" displayName="Table112" ref="C3:D20" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{F8107C66-607B-4058-88D5-7E54DAB777F3}" name="Table112" displayName="Table112" ref="C3:D20" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <autoFilter ref="C3:D20" xr:uid="{F8107C66-607B-4058-88D5-7E54DAB777F3}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{3CB6871F-D1D5-406A-A5F6-6C3D55F08377}" name="R#" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{4EAFD1C8-470F-415F-8511-C74AAEBC13D5}" name="Requirement" dataDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{3CB6871F-D1D5-406A-A5F6-6C3D55F08377}" name="R#" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{4EAFD1C8-470F-415F-8511-C74AAEBC13D5}" name="Requirement" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{3ABBEBA9-0A73-4764-B21E-B89DEA853C72}" name="Table213" displayName="Table213" ref="A61:N88" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" headerRowBorderDxfId="20" headerRowCellStyle="Heading 1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{3ABBEBA9-0A73-4764-B21E-B89DEA853C72}" name="Table213" displayName="Table213" ref="A61:N88" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15" headerRowCellStyle="Heading 1">
   <autoFilter ref="A61:N88" xr:uid="{3ABBEBA9-0A73-4764-B21E-B89DEA853C72}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A62:N104">
     <sortCondition ref="B1:B44"/>
   </sortState>
   <tableColumns count="14">
-    <tableColumn id="13" xr3:uid="{F3FFF02B-2482-42E9-B584-8F4D96166CA9}" name="Test Suite" dataDxfId="15"/>
-    <tableColumn id="11" xr3:uid="{1FB81E90-5ADA-4A56-88E3-E9B7D133719D}" name="Test Case No." dataDxfId="14"/>
-    <tableColumn id="1" xr3:uid="{0241E09D-793F-44A7-B410-7D90C214292F}" name="R No." dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{C02C19C0-E85F-4B0D-9246-CEF8EEF91981}" name="Scenario No." dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{D06ABCE0-F28E-4D7C-A949-E93075902232}" name="Test Decription" dataDxfId="11"/>
-    <tableColumn id="14" xr3:uid="{25B688DF-563E-4077-9340-7112817C8A39}" name="Interface" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{065BAE68-A3D8-4003-AD54-4BFAFFAE8D78}" name="Pre-requisites" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{0F72F42F-2308-4A45-A9BB-DA60FBC6FE2C}" name="Test Steps" dataDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{3DF66932-C56F-4194-BF09-A7E4A2C41CC5}" name="Test Data" dataDxfId="7"/>
-    <tableColumn id="8" xr3:uid="{B8964114-923E-4588-A3C3-4C6FD4E8B523}" name="Expected Results" dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{D3CA6EED-7389-48FF-A0B4-A7012E5844C3}" name="Actual Results" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{BE9DFA11-ED6D-4049-A2E2-267CB763A2C8}" name="Post Conditions" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{E0BDA9F2-509F-4DA0-9845-C87731E235F2}" name="Pass/Fail" dataDxfId="3"/>
-    <tableColumn id="12" xr3:uid="{C0F69B75-B8DE-4212-944C-F980F5FE35FB}" name="Comments" dataDxfId="2"/>
+    <tableColumn id="13" xr3:uid="{F3FFF02B-2482-42E9-B584-8F4D96166CA9}" name="Test Suite" dataDxfId="13"/>
+    <tableColumn id="11" xr3:uid="{1FB81E90-5ADA-4A56-88E3-E9B7D133719D}" name="Test Case No." dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{0241E09D-793F-44A7-B410-7D90C214292F}" name="R No." dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{C02C19C0-E85F-4B0D-9246-CEF8EEF91981}" name="Scenario No." dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{D06ABCE0-F28E-4D7C-A949-E93075902232}" name="Test Decription" dataDxfId="9"/>
+    <tableColumn id="14" xr3:uid="{25B688DF-563E-4077-9340-7112817C8A39}" name="Interface" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{065BAE68-A3D8-4003-AD54-4BFAFFAE8D78}" name="Pre-requisites" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{0F72F42F-2308-4A45-A9BB-DA60FBC6FE2C}" name="Test Steps" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{3DF66932-C56F-4194-BF09-A7E4A2C41CC5}" name="Test Data" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{B8964114-923E-4588-A3C3-4C6FD4E8B523}" name="Expected Results" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{D3CA6EED-7389-48FF-A0B4-A7012E5844C3}" name="Actual Results" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{BE9DFA11-ED6D-4049-A2E2-267CB763A2C8}" name="Post Conditions" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{E0BDA9F2-509F-4DA0-9845-C87731E235F2}" name="Pass/Fail" dataDxfId="1"/>
+    <tableColumn id="12" xr3:uid="{C0F69B75-B8DE-4212-944C-F980F5FE35FB}" name="Comments" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1718,14 +1758,14 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5FA4E805-D57D-4D43-9E0B-5E331A6D663E}" name="Table14" displayName="Table14" ref="D11:H30" totalsRowShown="0" dataDxfId="39" headerRowCellStyle="Heading 2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5FA4E805-D57D-4D43-9E0B-5E331A6D663E}" name="Table14" displayName="Table14" ref="D11:H30" totalsRowShown="0" dataDxfId="44" headerRowCellStyle="Heading 2">
   <autoFilter ref="D11:H30" xr:uid="{5FA4E805-D57D-4D43-9E0B-5E331A6D663E}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{BB1AF20A-CAB4-4CAB-81A5-CCAF14E79FE3}" name="Requirements" dataDxfId="44"/>
-    <tableColumn id="2" xr3:uid="{4DDE8730-E55A-4A81-BB34-A3E37063B965}" name="Description" dataDxfId="43"/>
-    <tableColumn id="3" xr3:uid="{F3723AD1-E0EE-4DAC-9210-7176FAFCDB41}" name="User Stories/Scenarios" dataDxfId="42"/>
-    <tableColumn id="4" xr3:uid="{7DE1817D-340D-4D60-8755-7170363B6042}" name="Notes" dataDxfId="41"/>
-    <tableColumn id="5" xr3:uid="{98DCC91C-BCC8-4706-B1E4-66C4499EBEB7}" name="Affected Systems" dataDxfId="40"/>
+    <tableColumn id="1" xr3:uid="{BB1AF20A-CAB4-4CAB-81A5-CCAF14E79FE3}" name="Requirements" dataDxfId="43"/>
+    <tableColumn id="2" xr3:uid="{4DDE8730-E55A-4A81-BB34-A3E37063B965}" name="Description" dataDxfId="42"/>
+    <tableColumn id="3" xr3:uid="{F3723AD1-E0EE-4DAC-9210-7176FAFCDB41}" name="User Stories/Scenarios" dataDxfId="41"/>
+    <tableColumn id="4" xr3:uid="{7DE1817D-340D-4D60-8755-7170363B6042}" name="Notes" dataDxfId="40"/>
+    <tableColumn id="5" xr3:uid="{98DCC91C-BCC8-4706-B1E4-66C4499EBEB7}" name="Affected Systems" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1754,14 +1794,14 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{90DF5E57-F0F7-4FA0-8DE8-33E1F966054E}" name="Table16" displayName="Table16" ref="D11:H30" totalsRowShown="0" dataDxfId="33" headerRowCellStyle="Heading 2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{90DF5E57-F0F7-4FA0-8DE8-33E1F966054E}" name="Table16" displayName="Table16" ref="D11:H30" totalsRowShown="0" dataDxfId="38" headerRowCellStyle="Heading 2">
   <autoFilter ref="D11:H30" xr:uid="{90DF5E57-F0F7-4FA0-8DE8-33E1F966054E}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{46746041-5C2F-4000-B825-78DCEE5C7F5D}" name="Requirements" dataDxfId="38"/>
-    <tableColumn id="2" xr3:uid="{A2917C86-AE50-404F-B2E2-45D77DB803DB}" name="Description" dataDxfId="37"/>
-    <tableColumn id="3" xr3:uid="{5BDBE60B-9C74-440C-960D-6FF584AAF1CC}" name="User Stories/Scenarios" dataDxfId="36"/>
-    <tableColumn id="4" xr3:uid="{403A2FD3-FDB5-4EB3-881D-3777DE4FBE4E}" name="Notes" dataDxfId="35"/>
-    <tableColumn id="5" xr3:uid="{B1A66192-CECE-4C07-A94F-0B1DD4A33300}" name="Affected Systems" dataDxfId="34"/>
+    <tableColumn id="1" xr3:uid="{46746041-5C2F-4000-B825-78DCEE5C7F5D}" name="Requirements" dataDxfId="37"/>
+    <tableColumn id="2" xr3:uid="{A2917C86-AE50-404F-B2E2-45D77DB803DB}" name="Description" dataDxfId="36"/>
+    <tableColumn id="3" xr3:uid="{5BDBE60B-9C74-440C-960D-6FF584AAF1CC}" name="User Stories/Scenarios" dataDxfId="35"/>
+    <tableColumn id="4" xr3:uid="{403A2FD3-FDB5-4EB3-881D-3777DE4FBE4E}" name="Notes" dataDxfId="34"/>
+    <tableColumn id="5" xr3:uid="{B1A66192-CECE-4C07-A94F-0B1DD4A33300}" name="Affected Systems" dataDxfId="33"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1790,14 +1830,14 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{A611E60F-4F24-4EB3-8CDC-8BBB573550F0}" name="Table18" displayName="Table18" ref="D11:H30" totalsRowShown="0" dataDxfId="27" headerRowCellStyle="Heading 2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{A611E60F-4F24-4EB3-8CDC-8BBB573550F0}" name="Table18" displayName="Table18" ref="D11:H30" totalsRowShown="0" dataDxfId="32" headerRowCellStyle="Heading 2">
   <autoFilter ref="D11:H30" xr:uid="{A611E60F-4F24-4EB3-8CDC-8BBB573550F0}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{E7FF2F9A-AB1C-4193-B154-F0080371199F}" name="Requirements" dataDxfId="32"/>
-    <tableColumn id="2" xr3:uid="{05F92AD7-E08F-4A7B-8CD0-5AD6A6659F64}" name="Description" dataDxfId="31"/>
-    <tableColumn id="3" xr3:uid="{52E9F203-1862-4583-8088-FB60845FE8FF}" name="User Stories/Scenarios" dataDxfId="30"/>
-    <tableColumn id="4" xr3:uid="{319355A8-A488-4D7D-89B7-E25B1E3092E4}" name="Notes" dataDxfId="29"/>
-    <tableColumn id="5" xr3:uid="{84602B21-3F71-4BC1-A799-E4208D2D39A4}" name="Affected Systems" dataDxfId="28"/>
+    <tableColumn id="1" xr3:uid="{E7FF2F9A-AB1C-4193-B154-F0080371199F}" name="Requirements" dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{05F92AD7-E08F-4A7B-8CD0-5AD6A6659F64}" name="Description" dataDxfId="30"/>
+    <tableColumn id="3" xr3:uid="{52E9F203-1862-4583-8088-FB60845FE8FF}" name="User Stories/Scenarios" dataDxfId="29"/>
+    <tableColumn id="4" xr3:uid="{319355A8-A488-4D7D-89B7-E25B1E3092E4}" name="Notes" dataDxfId="28"/>
+    <tableColumn id="5" xr3:uid="{84602B21-3F71-4BC1-A799-E4208D2D39A4}" name="Affected Systems" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1826,14 +1866,14 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{99C0BC7D-645F-4D4D-8BF0-B7A914E8F15D}" name="Table110" displayName="Table110" ref="D11:H30" totalsRowShown="0" dataDxfId="21" headerRowCellStyle="Heading 2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{99C0BC7D-645F-4D4D-8BF0-B7A914E8F15D}" name="Table110" displayName="Table110" ref="D11:H30" totalsRowShown="0" dataDxfId="26" headerRowCellStyle="Heading 2">
   <autoFilter ref="D11:H30" xr:uid="{99C0BC7D-645F-4D4D-8BF0-B7A914E8F15D}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{246CB3CD-654F-4B86-AF12-B19A107142F8}" name="Requirements" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{663BD34F-A7D9-450A-920D-FE75EDE33F04}" name="Description" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{9DBD0301-DDD7-471D-B108-491ADD7E6356}" name="User Stories/Scenarios" dataDxfId="24"/>
-    <tableColumn id="4" xr3:uid="{904A52D0-E01F-4764-9605-DF8BAB3F1860}" name="Notes" dataDxfId="23"/>
-    <tableColumn id="5" xr3:uid="{139A7663-409F-4E01-AE76-E84F213827DF}" name="Affected Systems" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{246CB3CD-654F-4B86-AF12-B19A107142F8}" name="Requirements" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{663BD34F-A7D9-450A-920D-FE75EDE33F04}" name="Description" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{9DBD0301-DDD7-471D-B108-491ADD7E6356}" name="User Stories/Scenarios" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{904A52D0-E01F-4764-9605-DF8BAB3F1860}" name="Notes" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{139A7663-409F-4E01-AE76-E84F213827DF}" name="Affected Systems" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2112,31 +2152,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" customWidth="1"/>
-    <col min="2" max="2" width="36.7109375" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" customWidth="1"/>
-    <col min="5" max="5" width="68.42578125" customWidth="1"/>
-    <col min="6" max="6" width="29.5703125" customWidth="1"/>
+    <col min="1" max="1" width="21.86328125" customWidth="1"/>
+    <col min="2" max="2" width="36.73046875" customWidth="1"/>
+    <col min="3" max="3" width="22.86328125" customWidth="1"/>
+    <col min="4" max="4" width="20.1328125" customWidth="1"/>
+    <col min="5" max="5" width="68.3984375" customWidth="1"/>
+    <col min="6" max="6" width="60.265625" customWidth="1"/>
     <col min="7" max="7" width="34" customWidth="1"/>
-    <col min="8" max="8" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.3984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.86328125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.1328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.1328125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="18" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.3984375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2147,7 +2187,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2158,7 +2198,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2166,12 +2206,12 @@
         <v>267</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="D11" s="1" t="s">
         <v>5</v>
       </c>
@@ -2188,51 +2228,61 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="43.15" thickTop="1" x14ac:dyDescent="0.45">
       <c r="D12" s="5">
         <v>1</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F12" s="5"/>
+      <c r="F12" s="5" t="s">
+        <v>268</v>
+      </c>
       <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-    </row>
-    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="H12" s="5" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="D13" s="5">
         <v>2</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F13" s="5"/>
+      <c r="F13" s="5" t="s">
+        <v>270</v>
+      </c>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D14" s="5">
         <v>3</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F14" s="5"/>
+      <c r="F14" s="5" t="s">
+        <v>271</v>
+      </c>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="D15" s="5">
         <v>4</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F15" s="5"/>
+      <c r="F15" s="5" t="s">
+        <v>272</v>
+      </c>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D16" s="5">
         <v>5</v>
       </c>
@@ -2243,7 +2293,7 @@
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="4:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="D17" s="5">
         <v>6</v>
       </c>
@@ -2254,91 +2304,91 @@
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
     </row>
-    <row r="18" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
     </row>
-    <row r="19" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
     </row>
-    <row r="20" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
     </row>
-    <row r="21" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
     </row>
-    <row r="22" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
     </row>
-    <row r="23" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
     </row>
-    <row r="24" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
     </row>
-    <row r="25" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
     </row>
-    <row r="26" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
     </row>
-    <row r="27" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
     </row>
-    <row r="28" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
     </row>
-    <row r="29" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
     </row>
-    <row r="39" spans="4:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="4:16" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="D39" s="1" t="s">
         <v>10</v>
       </c>
@@ -2379,12 +2429,13 @@
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="4:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="4:16" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="2">
-    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2397,26 +2448,26 @@
       <selection activeCell="B1" sqref="B1:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="2" max="2" width="34.5703125" customWidth="1"/>
-    <col min="3" max="3" width="36.85546875" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.3984375" customWidth="1"/>
+    <col min="2" max="2" width="34.59765625" customWidth="1"/>
+    <col min="3" max="3" width="36.86328125" customWidth="1"/>
+    <col min="4" max="4" width="20.59765625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="53" customWidth="1"/>
-    <col min="6" max="6" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.86328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.1328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.3984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.86328125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.1328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.1328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.3984375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2427,7 +2478,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2435,7 +2486,7 @@
         <v>44691</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2443,12 +2494,12 @@
         <v>267</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="D11" s="1" t="s">
         <v>5</v>
       </c>
@@ -2465,7 +2516,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="28.9" thickTop="1" x14ac:dyDescent="0.45">
       <c r="D12" s="5">
         <v>1</v>
       </c>
@@ -2476,7 +2527,7 @@
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
     </row>
-    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="D13" s="5">
         <v>2</v>
       </c>
@@ -2487,7 +2538,7 @@
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D14" s="5">
         <v>3</v>
       </c>
@@ -2498,7 +2549,7 @@
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="D15" s="5">
         <v>4</v>
       </c>
@@ -2509,7 +2560,7 @@
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="D16" s="5">
         <v>5</v>
       </c>
@@ -2520,7 +2571,7 @@
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="4:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="D17" s="5">
         <v>6</v>
       </c>
@@ -2531,98 +2582,98 @@
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
     </row>
-    <row r="18" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
     </row>
-    <row r="19" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
     </row>
-    <row r="20" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
     </row>
-    <row r="21" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
     </row>
-    <row r="22" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
     </row>
-    <row r="23" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
     </row>
-    <row r="24" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
     </row>
-    <row r="25" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
     </row>
-    <row r="26" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
     </row>
-    <row r="27" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
     </row>
-    <row r="28" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
     </row>
-    <row r="29" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
     </row>
-    <row r="30" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
     </row>
-    <row r="39" spans="4:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="4:16" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="D39" s="1" t="s">
         <v>10</v>
       </c>
@@ -2663,7 +2714,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="4:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="4:16" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="2">
@@ -2681,27 +2732,27 @@
       <selection activeCell="B1" sqref="B1:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" customWidth="1"/>
+    <col min="1" max="1" width="27.73046875" customWidth="1"/>
+    <col min="2" max="2" width="24.73046875" customWidth="1"/>
     <col min="3" max="3" width="44" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="63.5703125" customWidth="1"/>
-    <col min="6" max="6" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.59765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="63.59765625" customWidth="1"/>
+    <col min="6" max="6" width="26.86328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.1328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.3984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.86328125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.1328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.1328125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="18" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.3984375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2712,7 +2763,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2720,7 +2771,7 @@
         <v>44691</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2728,12 +2779,12 @@
         <v>267</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="D11" s="1" t="s">
         <v>5</v>
       </c>
@@ -2750,7 +2801,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="28.9" thickTop="1" x14ac:dyDescent="0.45">
       <c r="D12" s="5">
         <v>1</v>
       </c>
@@ -2761,7 +2812,7 @@
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D13" s="5">
         <v>2</v>
       </c>
@@ -2772,7 +2823,7 @@
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D14" s="5">
         <v>3</v>
       </c>
@@ -2783,7 +2834,7 @@
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="D15" s="5">
         <v>4</v>
       </c>
@@ -2794,7 +2845,7 @@
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="D16" s="5">
         <v>5</v>
       </c>
@@ -2805,105 +2856,105 @@
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
     </row>
-    <row r="18" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
     </row>
-    <row r="19" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
     </row>
-    <row r="20" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
     </row>
-    <row r="21" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
     </row>
-    <row r="22" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
     </row>
-    <row r="23" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
     </row>
-    <row r="24" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
     </row>
-    <row r="25" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
     </row>
-    <row r="26" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
     </row>
-    <row r="27" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
     </row>
-    <row r="28" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
     </row>
-    <row r="29" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
     </row>
-    <row r="30" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
     </row>
-    <row r="39" spans="4:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="4:16" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="D39" s="1" t="s">
         <v>10</v>
       </c>
@@ -2944,7 +2995,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="4:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="4:16" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="2">
@@ -2962,25 +3013,25 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" customWidth="1"/>
-    <col min="2" max="2" width="49.5703125" customWidth="1"/>
-    <col min="4" max="4" width="40.5703125" customWidth="1"/>
-    <col min="5" max="5" width="75.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.28515625" customWidth="1"/>
+    <col min="1" max="1" width="30.265625" customWidth="1"/>
+    <col min="2" max="2" width="49.59765625" customWidth="1"/>
+    <col min="4" max="4" width="40.59765625" customWidth="1"/>
+    <col min="5" max="5" width="75.59765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.265625" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
-    <col min="8" max="8" width="25.5703125" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.59765625" customWidth="1"/>
+    <col min="9" max="9" width="17.86328125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.1328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.1328125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="18" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.3984375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2991,7 +3042,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2999,7 +3050,7 @@
         <v>44691</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -3007,12 +3058,12 @@
         <v>267</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="D11" s="1" t="s">
         <v>5</v>
       </c>
@@ -3029,7 +3080,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="D12" s="5">
         <v>1</v>
       </c>
@@ -3040,7 +3091,7 @@
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D13" s="5">
         <v>2</v>
       </c>
@@ -3051,7 +3102,7 @@
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D14" s="5">
         <v>3</v>
       </c>
@@ -3062,7 +3113,7 @@
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="D15" s="5">
         <v>4</v>
       </c>
@@ -3073,7 +3124,7 @@
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="D16" s="5">
         <v>5</v>
       </c>
@@ -3084,105 +3135,105 @@
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
     </row>
-    <row r="18" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
     </row>
-    <row r="19" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
     </row>
-    <row r="20" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
     </row>
-    <row r="21" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
     </row>
-    <row r="22" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
     </row>
-    <row r="23" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
     </row>
-    <row r="24" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
     </row>
-    <row r="25" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
     </row>
-    <row r="26" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
     </row>
-    <row r="27" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
     </row>
-    <row r="28" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
     </row>
-    <row r="29" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
     </row>
-    <row r="30" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
     </row>
-    <row r="39" spans="4:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="4:16" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="D39" s="1" t="s">
         <v>10</v>
       </c>
@@ -3223,7 +3274,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="4:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="4:16" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="2">
@@ -3241,27 +3292,27 @@
       <selection activeCell="D54" sqref="D54:P54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.140625" customWidth="1"/>
-    <col min="3" max="3" width="28.5703125" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="75.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.1328125" customWidth="1"/>
+    <col min="3" max="3" width="28.59765625" customWidth="1"/>
+    <col min="4" max="4" width="20.59765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="75.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.86328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.1328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.3984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.86328125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.1328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.1328125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="18" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.3984375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -3272,7 +3323,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3280,7 +3331,7 @@
         <v>44691</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -3288,12 +3339,12 @@
         <v>267</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="D11" s="1" t="s">
         <v>5</v>
       </c>
@@ -3310,7 +3361,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="D12" s="5">
         <v>1</v>
       </c>
@@ -3321,7 +3372,7 @@
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D13" s="5">
         <v>2</v>
       </c>
@@ -3332,7 +3383,7 @@
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D14" s="5">
         <v>3</v>
       </c>
@@ -3343,7 +3394,7 @@
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D15" s="5">
         <v>4</v>
       </c>
@@ -3354,7 +3405,7 @@
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="D16" s="5">
         <v>5</v>
       </c>
@@ -3365,105 +3416,105 @@
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
     </row>
-    <row r="18" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
     </row>
-    <row r="19" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
     </row>
-    <row r="20" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
     </row>
-    <row r="21" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
     </row>
-    <row r="22" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
     </row>
-    <row r="23" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
     </row>
-    <row r="24" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
     </row>
-    <row r="25" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
     </row>
-    <row r="26" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
     </row>
-    <row r="27" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
     </row>
-    <row r="28" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
     </row>
-    <row r="29" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
     </row>
-    <row r="30" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
     </row>
-    <row r="39" spans="4:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="4:16" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="D39" s="1" t="s">
         <v>10</v>
       </c>
@@ -3504,7 +3555,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="4:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="4:16" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="2">
@@ -3518,30 +3569,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB450DC3-9D44-4E5F-88D4-527701B3D801}">
   <dimension ref="A3:N87"/>
   <sheetViews>
-    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+    <sheetView topLeftCell="J1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
       <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="84.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="84.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="255.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="95.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="105.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="255.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="115.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.86328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="255.73046875" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="95.1328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.3984375" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="105.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="255.73046875" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="115.1328125" style="7" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="232" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="222.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="69.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="26.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="84.140625" style="7"/>
+    <col min="11" max="11" width="222.265625" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="69.1328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.73046875" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="84.1328125" style="7"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:11" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="3:11" ht="25.9" thickBot="1" x14ac:dyDescent="0.8">
       <c r="C3" s="6" t="s">
         <v>52</v>
       </c>
@@ -3561,7 +3612,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="3:11" ht="27" thickTop="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="3:11" ht="25.9" thickTop="1" x14ac:dyDescent="0.75">
       <c r="C4" s="6" t="s">
         <v>54</v>
       </c>
@@ -3581,7 +3632,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="3:11" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="5" spans="3:11" ht="25.5" x14ac:dyDescent="0.75">
       <c r="C5" s="6" t="s">
         <v>56</v>
       </c>
@@ -3601,7 +3652,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="3:11" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="6" spans="3:11" ht="25.5" x14ac:dyDescent="0.75">
       <c r="C6" s="6" t="s">
         <v>58</v>
       </c>
@@ -3621,7 +3672,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="3:11" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="7" spans="3:11" ht="25.5" x14ac:dyDescent="0.75">
       <c r="C7" s="6" t="s">
         <v>60</v>
       </c>
@@ -3641,7 +3692,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="3:11" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="8" spans="3:11" ht="25.5" x14ac:dyDescent="0.75">
       <c r="C8" s="6" t="s">
         <v>62</v>
       </c>
@@ -3661,7 +3712,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="9" spans="3:11" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="9" spans="3:11" ht="25.5" x14ac:dyDescent="0.75">
       <c r="C9" s="6" t="s">
         <v>64</v>
       </c>
@@ -3681,7 +3732,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="3:11" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="10" spans="3:11" ht="25.5" x14ac:dyDescent="0.75">
       <c r="C10" s="6" t="s">
         <v>66</v>
       </c>
@@ -3701,7 +3752,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="11" spans="3:11" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="11" spans="3:11" ht="25.5" x14ac:dyDescent="0.75">
       <c r="C11" s="6" t="s">
         <v>68</v>
       </c>
@@ -3721,7 +3772,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="12" spans="3:11" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="12" spans="3:11" ht="25.5" x14ac:dyDescent="0.75">
       <c r="C12" s="6" t="s">
         <v>70</v>
       </c>
@@ -3741,7 +3792,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="13" spans="3:11" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="13" spans="3:11" ht="25.5" x14ac:dyDescent="0.75">
       <c r="C13" s="6" t="s">
         <v>72</v>
       </c>
@@ -3761,7 +3812,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="14" spans="3:11" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="14" spans="3:11" ht="25.5" x14ac:dyDescent="0.75">
       <c r="C14" s="6" t="s">
         <v>74</v>
       </c>
@@ -3781,7 +3832,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="15" spans="3:11" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="15" spans="3:11" ht="25.5" x14ac:dyDescent="0.75">
       <c r="C15" s="6" t="s">
         <v>76</v>
       </c>
@@ -3801,7 +3852,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="16" spans="3:11" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="16" spans="3:11" ht="25.5" x14ac:dyDescent="0.75">
       <c r="C16" s="6" t="s">
         <v>78</v>
       </c>
@@ -3821,7 +3872,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="17" spans="3:11" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="17" spans="3:11" ht="25.5" x14ac:dyDescent="0.75">
       <c r="C17" s="6" t="s">
         <v>80</v>
       </c>
@@ -3841,7 +3892,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="18" spans="3:11" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="18" spans="3:11" ht="25.5" x14ac:dyDescent="0.75">
       <c r="C18" s="6" t="s">
         <v>82</v>
       </c>
@@ -3861,7 +3912,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="19" spans="3:11" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="19" spans="3:11" ht="25.5" x14ac:dyDescent="0.75">
       <c r="C19" s="6" t="s">
         <v>84</v>
       </c>
@@ -3881,7 +3932,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="20" spans="3:11" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="20" spans="3:11" ht="25.5" x14ac:dyDescent="0.75">
       <c r="C20" s="6" t="s">
         <v>86</v>
       </c>
@@ -3901,7 +3952,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="21" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:11" x14ac:dyDescent="0.45">
       <c r="H21" s="16">
         <v>18</v>
       </c>
@@ -3915,7 +3966,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="22" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:11" x14ac:dyDescent="0.45">
       <c r="H22" s="16">
         <v>19</v>
       </c>
@@ -3929,7 +3980,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="23" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:11" x14ac:dyDescent="0.45">
       <c r="H23" s="17">
         <v>20</v>
       </c>
@@ -3943,7 +3994,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="24" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:11" x14ac:dyDescent="0.45">
       <c r="H24" s="10">
         <v>21</v>
       </c>
@@ -3957,7 +4008,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="61" spans="1:14" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:14" ht="25.9" thickBot="1" x14ac:dyDescent="0.8">
       <c r="A61" s="19" t="s">
         <v>141</v>
       </c>
@@ -4001,7 +4052,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="62" spans="1:14" ht="19.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" ht="18.399999999999999" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A62" s="7" t="s">
         <v>143</v>
       </c>
@@ -4035,7 +4086,7 @@
       <c r="M62" s="24"/>
       <c r="N62" s="24"/>
     </row>
-    <row r="63" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" ht="18" x14ac:dyDescent="0.45">
       <c r="A63" s="7" t="s">
         <v>143</v>
       </c>
@@ -4069,7 +4120,7 @@
       <c r="M63" s="24"/>
       <c r="N63" s="24"/>
     </row>
-    <row r="64" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" ht="18" x14ac:dyDescent="0.45">
       <c r="A64" s="7" t="s">
         <v>154</v>
       </c>
@@ -4105,7 +4156,7 @@
       <c r="M64" s="24"/>
       <c r="N64" s="24"/>
     </row>
-    <row r="65" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" ht="18" x14ac:dyDescent="0.45">
       <c r="A65" s="7" t="s">
         <v>143</v>
       </c>
@@ -4139,7 +4190,7 @@
       <c r="M65" s="24"/>
       <c r="N65" s="24"/>
     </row>
-    <row r="66" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" ht="18" x14ac:dyDescent="0.45">
       <c r="A66" s="7" t="s">
         <v>143</v>
       </c>
@@ -4173,7 +4224,7 @@
       <c r="M66" s="24"/>
       <c r="N66" s="24"/>
     </row>
-    <row r="67" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" ht="18" x14ac:dyDescent="0.45">
       <c r="A67" s="7" t="s">
         <v>143</v>
       </c>
@@ -4207,7 +4258,7 @@
       <c r="M67" s="24"/>
       <c r="N67" s="24"/>
     </row>
-    <row r="68" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" ht="18" x14ac:dyDescent="0.45">
       <c r="A68" s="7" t="s">
         <v>143</v>
       </c>
@@ -4249,7 +4300,7 @@
       </c>
       <c r="N68" s="24"/>
     </row>
-    <row r="69" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" ht="18" x14ac:dyDescent="0.45">
       <c r="A69" s="7" t="s">
         <v>154</v>
       </c>
@@ -4291,7 +4342,7 @@
       </c>
       <c r="N69" s="24"/>
     </row>
-    <row r="70" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" ht="18" x14ac:dyDescent="0.45">
       <c r="A70" s="7" t="s">
         <v>186</v>
       </c>
@@ -4331,7 +4382,7 @@
       </c>
       <c r="N70" s="24"/>
     </row>
-    <row r="71" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" ht="18" x14ac:dyDescent="0.45">
       <c r="A71" s="7" t="s">
         <v>193</v>
       </c>
@@ -4373,7 +4424,7 @@
       </c>
       <c r="N71" s="24"/>
     </row>
-    <row r="72" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" ht="18" x14ac:dyDescent="0.45">
       <c r="A72" s="7" t="s">
         <v>186</v>
       </c>
@@ -4415,7 +4466,7 @@
       </c>
       <c r="N72" s="24"/>
     </row>
-    <row r="73" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" ht="18" x14ac:dyDescent="0.45">
       <c r="A73" s="7" t="s">
         <v>193</v>
       </c>
@@ -4457,7 +4508,7 @@
       </c>
       <c r="N73" s="24"/>
     </row>
-    <row r="74" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14" ht="18" x14ac:dyDescent="0.45">
       <c r="A74" s="7" t="s">
         <v>143</v>
       </c>
@@ -4491,7 +4542,7 @@
       <c r="M74" s="24"/>
       <c r="N74" s="24"/>
     </row>
-    <row r="75" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:14" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="7" t="s">
         <v>143</v>
       </c>
@@ -4523,7 +4574,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="76" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:14" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="7" t="s">
         <v>154</v>
       </c>
@@ -4561,7 +4612,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="77" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:14" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="7" t="s">
         <v>193</v>
       </c>
@@ -4587,7 +4638,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="78" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:14" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="7" t="s">
         <v>193</v>
       </c>
@@ -4613,7 +4664,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="79" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:14" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="7" t="s">
         <v>193</v>
       </c>
@@ -4648,7 +4699,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="80" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:14" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="7" t="s">
         <v>193</v>
       </c>
@@ -4677,7 +4728,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:10" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="7" t="s">
         <v>193</v>
       </c>
@@ -4706,7 +4757,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="82" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:10" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="7" t="s">
         <v>193</v>
       </c>
@@ -4732,7 +4783,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="83" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:10" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="30" t="s">
         <v>143</v>
       </c>
@@ -4758,7 +4809,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="84" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:10" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="7" t="s">
         <v>193</v>
       </c>
@@ -4787,7 +4838,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="85" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:10" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="7" t="s">
         <v>193</v>
       </c>
@@ -4816,7 +4867,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="86" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:10" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="30" t="s">
         <v>186</v>
       </c>
@@ -4842,7 +4893,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="87" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:10" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="7" t="s">
         <v>193</v>
       </c>

</xml_diff>

<commit_message>
Updated ReadME and requirements documentation
</commit_message>
<xml_diff>
--- a/requirements_design/HCS_Requirements_Documentation.xlsx
+++ b/requirements_design/HCS_Requirements_Documentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7975897b035f41c7/my_files/UVIC/ROCKETRY/UVicRocketry_GITHUB/Hybrid-Controls-System/requirements_design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="263" documentId="11_F25DC773A252ABDACC104806C9D97FB05ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E5AC490-5FE7-415D-AC4D-ED470D76A62C}"/>
+  <xr:revisionPtr revIDLastSave="276" documentId="11_F25DC773A252ABDACC104806C9D97FB05ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0F9BCE3C-3BA3-4456-A18C-A359E9D6A1CA}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="345" yWindow="4395" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="System" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="298">
   <si>
     <t>Date Changed</t>
   </si>
@@ -1142,12 +1142,87 @@
   <si>
     <t>As a user, I want the system to respond to my input as close to realtime as possible (especially when considering the ABORT command). (Given</t>
   </si>
+  <si>
+    <t>Valve Control</t>
+  </si>
+  <si>
+    <t>Using the UI, enter various valve states into the system asynchronously.</t>
+  </si>
+  <si>
+    <t>The actuator position should follow the commands within the appropriate latency period</t>
+  </si>
+  <si>
+    <t>Abort Sequence</t>
+  </si>
+  <si>
+    <t>Set the system to all possible states. At each state trigger the abort sequence.</t>
+  </si>
+  <si>
+    <t>The abort sequence should interrupt all action and cause the system to shut down safely and immediately.</t>
+  </si>
+  <si>
+    <t>Communication Disconnect</t>
+  </si>
+  <si>
+    <t>For each component in the control system, manually cause a disconnect in the chain of communication.</t>
+  </si>
+  <si>
+    <t>Within the timeout period, All subsystems should realize the disconnect and perform shutdown procedure.</t>
+  </si>
+  <si>
+    <t>Closed Loop Communication</t>
+  </si>
+  <si>
+    <t>Send all command types from the UI. Independently observe the input and output messages of each active control system device.</t>
+  </si>
+  <si>
+    <t>All devices should follow the 2 way communication procedure and confirm all received messages with the sender with appropriate timing.</t>
+  </si>
+  <si>
+    <t>Invalid Commands Rejection</t>
+  </si>
+  <si>
+    <t>From the UI, send commands to move valves to an unsafe or invalid state.</t>
+  </si>
+  <si>
+    <t>The system should reject the commands and inform the user of the attempt.</t>
+  </si>
+  <si>
+    <t>Igniter Sequence</t>
+  </si>
+  <si>
+    <t>Run the procedure for the igniter sequence.</t>
+  </si>
+  <si>
+    <t>The actuators should operate as expected.</t>
+  </si>
+  <si>
+    <t>General Debug and Blocking Test</t>
+  </si>
+  <si>
+    <t>Attempt to force the control system into a stalled or blocked state.</t>
+  </si>
+  <si>
+    <t>The control system should never enter a stalled state</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>Goal</t>
+  </si>
+  <si>
+    <t>This communication line uses a fiber optic cable and two ethernet-fiber optic nodes</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1242,6 +1317,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFD4D4D4"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -1291,7 +1378,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -1365,6 +1452,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1373,7 +1475,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2"/>
@@ -1417,6 +1519,12 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="4" builtinId="27"/>
@@ -1677,28 +1785,6 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{AC920B7D-4F5E-43C9-96D8-B00077D86D7D}" name="Table211" displayName="Table211" ref="D39:P59" totalsRowShown="0" headerRowCellStyle="Heading 2">
-  <autoFilter ref="D39:P59" xr:uid="{AC920B7D-4F5E-43C9-96D8-B00077D86D7D}"/>
-  <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{5F8BA313-CC83-46AD-99F1-D3CA3D8C7CE2}" name="Test Cases"/>
-    <tableColumn id="2" xr3:uid="{2E2529E2-3703-4B7C-A139-8C4C8EFF1925}" name="R No."/>
-    <tableColumn id="3" xr3:uid="{02450990-2DE7-42CF-BD57-0C48A776B41A}" name="Scenario No."/>
-    <tableColumn id="4" xr3:uid="{CE94C48A-8DE9-4B35-8B80-7120BE291144}" name="Test Decription"/>
-    <tableColumn id="5" xr3:uid="{223BD5AD-AAB3-40D5-9924-975E4E75AE4A}" name="Interface"/>
-    <tableColumn id="6" xr3:uid="{A3A484D1-0790-4ECC-90E3-DA2B3651BD9E}" name="Pre-requisites"/>
-    <tableColumn id="7" xr3:uid="{B639B154-9EC5-43F2-A02E-22C04DF327A8}" name="Test Steps"/>
-    <tableColumn id="8" xr3:uid="{CA64F9B4-628E-47A9-A79E-79EABBFE63FA}" name="Test Data"/>
-    <tableColumn id="9" xr3:uid="{D2BD0904-9592-44BB-A10A-EBA5E38EFE04}" name="Expected Results"/>
-    <tableColumn id="10" xr3:uid="{066FBEC0-2FBC-4497-ADE8-0DA8A0C2540F}" name="Actual Results"/>
-    <tableColumn id="11" xr3:uid="{4765B72E-C823-4FF8-BBA6-94A2CF622928}" name="Post Conditions"/>
-    <tableColumn id="12" xr3:uid="{08523F9E-CF17-4583-9157-7D1EA3809D9B}" name="Pass/Fail"/>
-    <tableColumn id="13" xr3:uid="{A7519F46-F84F-476F-9715-B7747F5B01DE}" name="Comments"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{F8107C66-607B-4058-88D5-7E54DAB777F3}" name="Table112" displayName="Table112" ref="C3:D20" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <autoFilter ref="C3:D20" xr:uid="{F8107C66-607B-4058-88D5-7E54DAB777F3}"/>
   <tableColumns count="2">
@@ -1709,7 +1795,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{3ABBEBA9-0A73-4764-B21E-B89DEA853C72}" name="Table213" displayName="Table213" ref="A61:N88" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15" headerRowCellStyle="Heading 1">
   <autoFilter ref="A61:N88" xr:uid="{3ABBEBA9-0A73-4764-B21E-B89DEA853C72}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A62:N104">
@@ -1736,28 +1822,6 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F4A1ED68-789E-41AA-B809-23E37228D0F1}" name="Table2" displayName="Table2" ref="D39:P59" totalsRowShown="0" headerRowCellStyle="Heading 2">
-  <autoFilter ref="D39:P59" xr:uid="{F4A1ED68-789E-41AA-B809-23E37228D0F1}"/>
-  <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{CDD9A311-A3F8-4492-8BE3-4E885E7E6511}" name="Test Cases"/>
-    <tableColumn id="2" xr3:uid="{92FEB540-BA66-46BD-9CD3-132FFB3090D3}" name="R No."/>
-    <tableColumn id="3" xr3:uid="{B49E6DE4-C16C-4AF6-AA9F-D68A02CCC62A}" name="Scenario No."/>
-    <tableColumn id="4" xr3:uid="{B8F705A3-C7F8-4613-B06A-E2CBC5FBD5AA}" name="Test Decription"/>
-    <tableColumn id="5" xr3:uid="{D9C94531-B1A9-4E47-BBD4-F44C09F7F4AA}" name="Interface"/>
-    <tableColumn id="6" xr3:uid="{234A4BD7-85F9-4F47-9B1B-7D01DCFADF42}" name="Pre-requisites"/>
-    <tableColumn id="7" xr3:uid="{0A9B9B3C-72B6-41AC-911F-96D097DBE570}" name="Test Steps"/>
-    <tableColumn id="8" xr3:uid="{94852BF5-7C2B-46B4-9EBB-9E3D7D3CD41A}" name="Test Data"/>
-    <tableColumn id="9" xr3:uid="{D24325E8-4C71-4E6D-8851-6E163C6E741D}" name="Expected Results"/>
-    <tableColumn id="10" xr3:uid="{F0E122E2-005D-4714-90AC-BC9036B9BEED}" name="Actual Results"/>
-    <tableColumn id="11" xr3:uid="{A28BF972-4EBF-49A2-848A-7CC482991915}" name="Post Conditions"/>
-    <tableColumn id="12" xr3:uid="{727CDB3F-7FB7-49EA-AC25-0BE4FE6791BB}" name="Pass/Fail"/>
-    <tableColumn id="13" xr3:uid="{052D7594-0B4B-4A60-B1F1-A11B264918C2}" name="Comments"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5FA4E805-D57D-4D43-9E0B-5E331A6D663E}" name="Table14" displayName="Table14" ref="D11:H30" totalsRowShown="0" dataDxfId="44" headerRowCellStyle="Heading 2">
   <autoFilter ref="D11:H30" xr:uid="{5FA4E805-D57D-4D43-9E0B-5E331A6D663E}"/>
   <tableColumns count="5">
@@ -1771,7 +1835,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E72C23B9-2964-4B53-98EE-7AF6DA61F8CA}" name="Table25" displayName="Table25" ref="D39:P59" totalsRowShown="0" headerRowCellStyle="Heading 2">
   <autoFilter ref="D39:P59" xr:uid="{E72C23B9-2964-4B53-98EE-7AF6DA61F8CA}"/>
   <tableColumns count="13">
@@ -1793,7 +1857,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{90DF5E57-F0F7-4FA0-8DE8-33E1F966054E}" name="Table16" displayName="Table16" ref="D11:H30" totalsRowShown="0" dataDxfId="38" headerRowCellStyle="Heading 2">
   <autoFilter ref="D11:H30" xr:uid="{90DF5E57-F0F7-4FA0-8DE8-33E1F966054E}"/>
   <tableColumns count="5">
@@ -1807,7 +1871,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{34380E41-180F-4ED1-96AD-C422C14E13A9}" name="Table27" displayName="Table27" ref="D39:P59" totalsRowShown="0" headerRowCellStyle="Heading 2">
   <autoFilter ref="D39:P59" xr:uid="{34380E41-180F-4ED1-96AD-C422C14E13A9}"/>
   <tableColumns count="13">
@@ -1829,7 +1893,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{A611E60F-4F24-4EB3-8CDC-8BBB573550F0}" name="Table18" displayName="Table18" ref="D11:H30" totalsRowShown="0" dataDxfId="32" headerRowCellStyle="Heading 2">
   <autoFilter ref="D11:H30" xr:uid="{A611E60F-4F24-4EB3-8CDC-8BBB573550F0}"/>
   <tableColumns count="5">
@@ -1843,7 +1907,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{E54182DD-5242-46BD-81F7-57A1EC0A1412}" name="Table29" displayName="Table29" ref="D39:P59" totalsRowShown="0" headerRowCellStyle="Heading 2">
   <autoFilter ref="D39:P59" xr:uid="{E54182DD-5242-46BD-81F7-57A1EC0A1412}"/>
   <tableColumns count="13">
@@ -1865,7 +1929,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{99C0BC7D-645F-4D4D-8BF0-B7A914E8F15D}" name="Table110" displayName="Table110" ref="D11:H30" totalsRowShown="0" dataDxfId="26" headerRowCellStyle="Heading 2">
   <autoFilter ref="D11:H30" xr:uid="{99C0BC7D-645F-4D4D-8BF0-B7A914E8F15D}"/>
   <tableColumns count="5">
@@ -1874,6 +1938,28 @@
     <tableColumn id="3" xr3:uid="{9DBD0301-DDD7-471D-B108-491ADD7E6356}" name="User Stories/Scenarios" dataDxfId="23"/>
     <tableColumn id="4" xr3:uid="{904A52D0-E01F-4764-9605-DF8BAB3F1860}" name="Notes" dataDxfId="22"/>
     <tableColumn id="5" xr3:uid="{139A7663-409F-4E01-AE76-E84F213827DF}" name="Affected Systems" dataDxfId="21"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{AC920B7D-4F5E-43C9-96D8-B00077D86D7D}" name="Table211" displayName="Table211" ref="D39:P59" totalsRowShown="0" headerRowCellStyle="Heading 2">
+  <autoFilter ref="D39:P59" xr:uid="{AC920B7D-4F5E-43C9-96D8-B00077D86D7D}"/>
+  <tableColumns count="13">
+    <tableColumn id="1" xr3:uid="{5F8BA313-CC83-46AD-99F1-D3CA3D8C7CE2}" name="Test Cases"/>
+    <tableColumn id="2" xr3:uid="{2E2529E2-3703-4B7C-A139-8C4C8EFF1925}" name="R No."/>
+    <tableColumn id="3" xr3:uid="{02450990-2DE7-42CF-BD57-0C48A776B41A}" name="Scenario No."/>
+    <tableColumn id="4" xr3:uid="{CE94C48A-8DE9-4B35-8B80-7120BE291144}" name="Test Decription"/>
+    <tableColumn id="5" xr3:uid="{223BD5AD-AAB3-40D5-9924-975E4E75AE4A}" name="Interface"/>
+    <tableColumn id="6" xr3:uid="{A3A484D1-0790-4ECC-90E3-DA2B3651BD9E}" name="Pre-requisites"/>
+    <tableColumn id="7" xr3:uid="{B639B154-9EC5-43F2-A02E-22C04DF327A8}" name="Test Steps"/>
+    <tableColumn id="8" xr3:uid="{CA64F9B4-628E-47A9-A79E-79EABBFE63FA}" name="Test Data"/>
+    <tableColumn id="9" xr3:uid="{D2BD0904-9592-44BB-A10A-EBA5E38EFE04}" name="Expected Results"/>
+    <tableColumn id="10" xr3:uid="{066FBEC0-2FBC-4497-ADE8-0DA8A0C2540F}" name="Actual Results"/>
+    <tableColumn id="11" xr3:uid="{4765B72E-C823-4FF8-BBA6-94A2CF622928}" name="Post Conditions"/>
+    <tableColumn id="12" xr3:uid="{08523F9E-CF17-4583-9157-7D1EA3809D9B}" name="Pass/Fail"/>
+    <tableColumn id="13" xr3:uid="{A7519F46-F84F-476F-9715-B7747F5B01DE}" name="Comments"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2150,33 +2236,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P40"/>
+  <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="C16" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.86328125" customWidth="1"/>
-    <col min="2" max="2" width="36.73046875" customWidth="1"/>
-    <col min="3" max="3" width="22.86328125" customWidth="1"/>
-    <col min="4" max="4" width="20.1328125" customWidth="1"/>
-    <col min="5" max="5" width="68.3984375" customWidth="1"/>
-    <col min="6" max="6" width="60.265625" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" customWidth="1"/>
+    <col min="2" max="2" width="36.7109375" customWidth="1"/>
+    <col min="3" max="3" width="45.5703125" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" customWidth="1"/>
+    <col min="5" max="5" width="68.42578125" customWidth="1"/>
+    <col min="6" max="6" width="60.28515625" customWidth="1"/>
     <col min="7" max="7" width="34" customWidth="1"/>
-    <col min="8" max="8" width="21.3984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.86328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.1328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.1328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="18" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.3984375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.59765625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2187,7 +2273,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2198,7 +2284,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2206,12 +2292,12 @@
         <v>267</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="11" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D11" s="1" t="s">
         <v>5</v>
       </c>
@@ -2228,7 +2314,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="43.15" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="D12" s="5">
         <v>1</v>
       </c>
@@ -2243,7 +2329,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="D13" s="5">
         <v>2</v>
       </c>
@@ -2256,7 +2342,7 @@
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D14" s="5">
         <v>3</v>
       </c>
@@ -2269,7 +2355,7 @@
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="D15" s="5">
         <v>4</v>
       </c>
@@ -2282,7 +2368,7 @@
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D16" s="5">
         <v>5</v>
       </c>
@@ -2293,7 +2379,7 @@
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="4:8" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D17" s="5">
         <v>6</v>
       </c>
@@ -2304,138 +2390,211 @@
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
     </row>
-    <row r="18" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
     </row>
-    <row r="19" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
     </row>
-    <row r="20" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
     </row>
-    <row r="21" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="32" t="s">
+        <v>297</v>
+      </c>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
     </row>
-    <row r="22" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
     </row>
-    <row r="23" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
     </row>
-    <row r="24" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
     </row>
-    <row r="25" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
     </row>
-    <row r="26" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
     </row>
-    <row r="27" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
     </row>
-    <row r="28" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
     </row>
-    <row r="29" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
     </row>
-    <row r="39" spans="4:16" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="D39" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H39" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I39" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J39" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K39" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L39" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="M39" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N39" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O39" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="P39" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="40" spans="4:16" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
+    <row r="39" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="40" spans="3:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C40" s="31" t="s">
+        <v>294</v>
+      </c>
+      <c r="D40" s="31" t="s">
+        <v>295</v>
+      </c>
+      <c r="E40" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="F40" s="31" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="41" spans="3:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C41" s="31" t="s">
+        <v>273</v>
+      </c>
+      <c r="D41" s="31">
+        <v>1</v>
+      </c>
+      <c r="E41" s="31" t="s">
+        <v>274</v>
+      </c>
+      <c r="F41" s="31" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="42" spans="3:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C42" s="31" t="s">
+        <v>276</v>
+      </c>
+      <c r="D42" s="31">
+        <v>2</v>
+      </c>
+      <c r="E42" s="31" t="s">
+        <v>277</v>
+      </c>
+      <c r="F42" s="31" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="43" spans="3:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C43" s="31" t="s">
+        <v>279</v>
+      </c>
+      <c r="D43" s="31">
+        <v>3</v>
+      </c>
+      <c r="E43" s="31" t="s">
+        <v>280</v>
+      </c>
+      <c r="F43" s="31" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="44" spans="3:6" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C44" s="31" t="s">
+        <v>282</v>
+      </c>
+      <c r="D44" s="31">
+        <v>4</v>
+      </c>
+      <c r="E44" s="31" t="s">
+        <v>283</v>
+      </c>
+      <c r="F44" s="31" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="45" spans="3:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C45" s="31" t="s">
+        <v>285</v>
+      </c>
+      <c r="D45" s="31">
+        <v>5</v>
+      </c>
+      <c r="E45" s="31" t="s">
+        <v>286</v>
+      </c>
+      <c r="F45" s="31" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="46" spans="3:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C46" s="31" t="s">
+        <v>288</v>
+      </c>
+      <c r="D46" s="31">
+        <v>6</v>
+      </c>
+      <c r="E46" s="31" t="s">
+        <v>289</v>
+      </c>
+      <c r="F46" s="31" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="47" spans="3:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C47" s="31" t="s">
+        <v>291</v>
+      </c>
+      <c r="D47" s="31">
+        <v>7</v>
+      </c>
+      <c r="E47" s="31" t="s">
+        <v>292</v>
+      </c>
+      <c r="F47" s="31" t="s">
+        <v>293</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <tableParts count="2">
+  <tableParts count="1">
     <tablePart r:id="rId2"/>
-    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2448,26 +2607,26 @@
       <selection activeCell="B1" sqref="B1:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.3984375" customWidth="1"/>
-    <col min="2" max="2" width="34.59765625" customWidth="1"/>
-    <col min="3" max="3" width="36.86328125" customWidth="1"/>
-    <col min="4" max="4" width="20.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="34.5703125" customWidth="1"/>
+    <col min="3" max="3" width="36.85546875" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="53" customWidth="1"/>
-    <col min="6" max="6" width="26.86328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.1328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.3984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.86328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.1328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.1328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.3984375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.59765625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2478,7 +2637,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2486,7 +2645,7 @@
         <v>44691</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2494,12 +2653,12 @@
         <v>267</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="11" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D11" s="1" t="s">
         <v>5</v>
       </c>
@@ -2516,7 +2675,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="28.9" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="D12" s="5">
         <v>1</v>
       </c>
@@ -2527,7 +2686,7 @@
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
     </row>
-    <row r="13" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D13" s="5">
         <v>2</v>
       </c>
@@ -2538,7 +2697,7 @@
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D14" s="5">
         <v>3</v>
       </c>
@@ -2549,7 +2708,7 @@
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D15" s="5">
         <v>4</v>
       </c>
@@ -2560,7 +2719,7 @@
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D16" s="5">
         <v>5</v>
       </c>
@@ -2571,7 +2730,7 @@
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="4:8" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="17" spans="4:8" ht="45" x14ac:dyDescent="0.25">
       <c r="D17" s="5">
         <v>6</v>
       </c>
@@ -2582,98 +2741,98 @@
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
     </row>
-    <row r="18" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
     </row>
-    <row r="19" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
     </row>
-    <row r="20" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="20" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
     </row>
-    <row r="21" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="21" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
     </row>
-    <row r="22" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="22" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
     </row>
-    <row r="23" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="23" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
     </row>
-    <row r="24" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="24" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
     </row>
-    <row r="25" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="25" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
     </row>
-    <row r="26" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="26" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
     </row>
-    <row r="27" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="27" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
     </row>
-    <row r="28" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="28" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
     </row>
-    <row r="29" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="29" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
     </row>
-    <row r="30" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="30" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
     </row>
-    <row r="39" spans="4:16" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="39" spans="4:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D39" s="1" t="s">
         <v>10</v>
       </c>
@@ -2714,7 +2873,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="4:16" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
+    <row r="40" spans="4:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="2">
@@ -2732,27 +2891,27 @@
       <selection activeCell="B1" sqref="B1:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.73046875" customWidth="1"/>
-    <col min="2" max="2" width="24.73046875" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" customWidth="1"/>
     <col min="3" max="3" width="44" customWidth="1"/>
-    <col min="4" max="4" width="20.59765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="63.59765625" customWidth="1"/>
-    <col min="6" max="6" width="26.86328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.1328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.3984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="63.5703125" customWidth="1"/>
+    <col min="6" max="6" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.1328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.1328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="18" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.3984375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.59765625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2763,7 +2922,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2771,7 +2930,7 @@
         <v>44691</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2779,12 +2938,12 @@
         <v>267</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="11" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D11" s="1" t="s">
         <v>5</v>
       </c>
@@ -2801,7 +2960,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="28.9" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="D12" s="5">
         <v>1</v>
       </c>
@@ -2812,7 +2971,7 @@
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D13" s="5">
         <v>2</v>
       </c>
@@ -2823,7 +2982,7 @@
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D14" s="5">
         <v>3</v>
       </c>
@@ -2834,7 +2993,7 @@
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D15" s="5">
         <v>4</v>
       </c>
@@ -2845,7 +3004,7 @@
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D16" s="5">
         <v>5</v>
       </c>
@@ -2856,105 +3015,105 @@
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
     </row>
-    <row r="18" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
     </row>
-    <row r="19" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
     </row>
-    <row r="20" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="20" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
     </row>
-    <row r="21" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="21" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
     </row>
-    <row r="22" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="22" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
     </row>
-    <row r="23" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="23" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
     </row>
-    <row r="24" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="24" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
     </row>
-    <row r="25" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="25" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
     </row>
-    <row r="26" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="26" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
     </row>
-    <row r="27" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="27" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
     </row>
-    <row r="28" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="28" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
     </row>
-    <row r="29" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="29" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
     </row>
-    <row r="30" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="30" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
     </row>
-    <row r="39" spans="4:16" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="39" spans="4:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D39" s="1" t="s">
         <v>10</v>
       </c>
@@ -2995,7 +3154,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="4:16" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
+    <row r="40" spans="4:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="2">
@@ -3013,25 +3172,25 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.265625" customWidth="1"/>
-    <col min="2" max="2" width="49.59765625" customWidth="1"/>
-    <col min="4" max="4" width="40.59765625" customWidth="1"/>
-    <col min="5" max="5" width="75.59765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.265625" customWidth="1"/>
+    <col min="1" max="1" width="30.28515625" customWidth="1"/>
+    <col min="2" max="2" width="49.5703125" customWidth="1"/>
+    <col min="4" max="4" width="40.5703125" customWidth="1"/>
+    <col min="5" max="5" width="75.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.28515625" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
-    <col min="8" max="8" width="25.59765625" customWidth="1"/>
-    <col min="9" max="9" width="17.86328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.5703125" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.1328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.1328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="18" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.3984375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.59765625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -3042,7 +3201,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3050,7 +3209,7 @@
         <v>44691</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -3058,12 +3217,12 @@
         <v>267</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="11" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D11" s="1" t="s">
         <v>5</v>
       </c>
@@ -3080,7 +3239,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="D12" s="5">
         <v>1</v>
       </c>
@@ -3091,7 +3250,7 @@
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D13" s="5">
         <v>2</v>
       </c>
@@ -3102,7 +3261,7 @@
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D14" s="5">
         <v>3</v>
       </c>
@@ -3113,7 +3272,7 @@
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D15" s="5">
         <v>4</v>
       </c>
@@ -3124,7 +3283,7 @@
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D16" s="5">
         <v>5</v>
       </c>
@@ -3135,105 +3294,105 @@
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
     </row>
-    <row r="18" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
     </row>
-    <row r="19" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
     </row>
-    <row r="20" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="20" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
     </row>
-    <row r="21" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="21" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
     </row>
-    <row r="22" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="22" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
     </row>
-    <row r="23" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="23" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
     </row>
-    <row r="24" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="24" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
     </row>
-    <row r="25" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="25" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
     </row>
-    <row r="26" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="26" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
     </row>
-    <row r="27" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="27" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
     </row>
-    <row r="28" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="28" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
     </row>
-    <row r="29" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="29" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
     </row>
-    <row r="30" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="30" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
     </row>
-    <row r="39" spans="4:16" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="39" spans="4:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D39" s="1" t="s">
         <v>10</v>
       </c>
@@ -3274,7 +3433,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="4:16" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
+    <row r="40" spans="4:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="2">
@@ -3292,27 +3451,27 @@
       <selection activeCell="D54" sqref="D54:P54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.73046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.1328125" customWidth="1"/>
-    <col min="3" max="3" width="28.59765625" customWidth="1"/>
-    <col min="4" max="4" width="20.59765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="75.73046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.86328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.1328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.3984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.86328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.140625" customWidth="1"/>
+    <col min="3" max="3" width="28.5703125" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="75.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.1328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.1328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="18" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.3984375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.59765625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -3323,7 +3482,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3331,7 +3490,7 @@
         <v>44691</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -3339,12 +3498,12 @@
         <v>267</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="11" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D11" s="1" t="s">
         <v>5</v>
       </c>
@@ -3361,7 +3520,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="D12" s="5">
         <v>1</v>
       </c>
@@ -3372,7 +3531,7 @@
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D13" s="5">
         <v>2</v>
       </c>
@@ -3383,7 +3542,7 @@
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D14" s="5">
         <v>3</v>
       </c>
@@ -3394,7 +3553,7 @@
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D15" s="5">
         <v>4</v>
       </c>
@@ -3405,7 +3564,7 @@
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D16" s="5">
         <v>5</v>
       </c>
@@ -3416,105 +3575,105 @@
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
     </row>
-    <row r="18" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
     </row>
-    <row r="19" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
     </row>
-    <row r="20" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="20" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
     </row>
-    <row r="21" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="21" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
     </row>
-    <row r="22" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="22" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
     </row>
-    <row r="23" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="23" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
     </row>
-    <row r="24" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="24" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
     </row>
-    <row r="25" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="25" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
     </row>
-    <row r="26" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="26" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
     </row>
-    <row r="27" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="27" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
     </row>
-    <row r="28" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="28" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
     </row>
-    <row r="29" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="29" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
     </row>
-    <row r="30" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="30" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
     </row>
-    <row r="39" spans="4:16" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="39" spans="4:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D39" s="1" t="s">
         <v>10</v>
       </c>
@@ -3555,7 +3714,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="4:16" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
+    <row r="40" spans="4:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="2">
@@ -3573,26 +3732,26 @@
       <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="84.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="84.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.86328125" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="255.73046875" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="95.1328125" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.3984375" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="105.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="255.73046875" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="115.1328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="255.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="95.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="105.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="255.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="115.140625" style="7" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="232" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="222.265625" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="69.1328125" style="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.73046875" style="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="26.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="84.1328125" style="7"/>
+    <col min="11" max="11" width="222.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="69.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="84.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:11" ht="25.9" thickBot="1" x14ac:dyDescent="0.8">
+    <row r="3" spans="3:11" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C3" s="6" t="s">
         <v>52</v>
       </c>
@@ -3612,7 +3771,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="3:11" ht="25.9" thickTop="1" x14ac:dyDescent="0.75">
+    <row r="4" spans="3:11" ht="27" thickTop="1" x14ac:dyDescent="0.4">
       <c r="C4" s="6" t="s">
         <v>54</v>
       </c>
@@ -3632,7 +3791,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="3:11" ht="25.5" x14ac:dyDescent="0.75">
+    <row r="5" spans="3:11" ht="26.25" x14ac:dyDescent="0.4">
       <c r="C5" s="6" t="s">
         <v>56</v>
       </c>
@@ -3652,7 +3811,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="3:11" ht="25.5" x14ac:dyDescent="0.75">
+    <row r="6" spans="3:11" ht="26.25" x14ac:dyDescent="0.4">
       <c r="C6" s="6" t="s">
         <v>58</v>
       </c>
@@ -3672,7 +3831,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="3:11" ht="25.5" x14ac:dyDescent="0.75">
+    <row r="7" spans="3:11" ht="26.25" x14ac:dyDescent="0.4">
       <c r="C7" s="6" t="s">
         <v>60</v>
       </c>
@@ -3692,7 +3851,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="3:11" ht="25.5" x14ac:dyDescent="0.75">
+    <row r="8" spans="3:11" ht="26.25" x14ac:dyDescent="0.4">
       <c r="C8" s="6" t="s">
         <v>62</v>
       </c>
@@ -3712,7 +3871,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="9" spans="3:11" ht="25.5" x14ac:dyDescent="0.75">
+    <row r="9" spans="3:11" ht="26.25" x14ac:dyDescent="0.4">
       <c r="C9" s="6" t="s">
         <v>64</v>
       </c>
@@ -3732,7 +3891,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="3:11" ht="25.5" x14ac:dyDescent="0.75">
+    <row r="10" spans="3:11" ht="26.25" x14ac:dyDescent="0.4">
       <c r="C10" s="6" t="s">
         <v>66</v>
       </c>
@@ -3752,7 +3911,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="11" spans="3:11" ht="25.5" x14ac:dyDescent="0.75">
+    <row r="11" spans="3:11" ht="26.25" x14ac:dyDescent="0.4">
       <c r="C11" s="6" t="s">
         <v>68</v>
       </c>
@@ -3772,7 +3931,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="12" spans="3:11" ht="25.5" x14ac:dyDescent="0.75">
+    <row r="12" spans="3:11" ht="26.25" x14ac:dyDescent="0.4">
       <c r="C12" s="6" t="s">
         <v>70</v>
       </c>
@@ -3792,7 +3951,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="13" spans="3:11" ht="25.5" x14ac:dyDescent="0.75">
+    <row r="13" spans="3:11" ht="26.25" x14ac:dyDescent="0.4">
       <c r="C13" s="6" t="s">
         <v>72</v>
       </c>
@@ -3812,7 +3971,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="14" spans="3:11" ht="25.5" x14ac:dyDescent="0.75">
+    <row r="14" spans="3:11" ht="26.25" x14ac:dyDescent="0.4">
       <c r="C14" s="6" t="s">
         <v>74</v>
       </c>
@@ -3832,7 +3991,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="15" spans="3:11" ht="25.5" x14ac:dyDescent="0.75">
+    <row r="15" spans="3:11" ht="26.25" x14ac:dyDescent="0.4">
       <c r="C15" s="6" t="s">
         <v>76</v>
       </c>
@@ -3852,7 +4011,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="16" spans="3:11" ht="25.5" x14ac:dyDescent="0.75">
+    <row r="16" spans="3:11" ht="26.25" x14ac:dyDescent="0.4">
       <c r="C16" s="6" t="s">
         <v>78</v>
       </c>
@@ -3872,7 +4031,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="17" spans="3:11" ht="25.5" x14ac:dyDescent="0.75">
+    <row r="17" spans="3:11" ht="26.25" x14ac:dyDescent="0.4">
       <c r="C17" s="6" t="s">
         <v>80</v>
       </c>
@@ -3892,7 +4051,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="18" spans="3:11" ht="25.5" x14ac:dyDescent="0.75">
+    <row r="18" spans="3:11" ht="26.25" x14ac:dyDescent="0.4">
       <c r="C18" s="6" t="s">
         <v>82</v>
       </c>
@@ -3912,7 +4071,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="19" spans="3:11" ht="25.5" x14ac:dyDescent="0.75">
+    <row r="19" spans="3:11" ht="26.25" x14ac:dyDescent="0.4">
       <c r="C19" s="6" t="s">
         <v>84</v>
       </c>
@@ -3932,7 +4091,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="20" spans="3:11" ht="25.5" x14ac:dyDescent="0.75">
+    <row r="20" spans="3:11" ht="26.25" x14ac:dyDescent="0.4">
       <c r="C20" s="6" t="s">
         <v>86</v>
       </c>
@@ -3952,7 +4111,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="21" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="21" spans="3:11" x14ac:dyDescent="0.25">
       <c r="H21" s="16">
         <v>18</v>
       </c>
@@ -3966,7 +4125,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="22" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="22" spans="3:11" x14ac:dyDescent="0.25">
       <c r="H22" s="16">
         <v>19</v>
       </c>
@@ -3980,7 +4139,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="23" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="23" spans="3:11" x14ac:dyDescent="0.25">
       <c r="H23" s="17">
         <v>20</v>
       </c>
@@ -3994,7 +4153,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="24" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="24" spans="3:11" x14ac:dyDescent="0.25">
       <c r="H24" s="10">
         <v>21</v>
       </c>
@@ -4008,7 +4167,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="61" spans="1:14" ht="25.9" thickBot="1" x14ac:dyDescent="0.8">
+    <row r="61" spans="1:14" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A61" s="19" t="s">
         <v>141</v>
       </c>
@@ -4052,7 +4211,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="62" spans="1:14" ht="18.399999999999999" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:14" ht="19.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
         <v>143</v>
       </c>
@@ -4086,7 +4245,7 @@
       <c r="M62" s="24"/>
       <c r="N62" s="24"/>
     </row>
-    <row r="63" spans="1:14" ht="18" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
         <v>143</v>
       </c>
@@ -4120,7 +4279,7 @@
       <c r="M63" s="24"/>
       <c r="N63" s="24"/>
     </row>
-    <row r="64" spans="1:14" ht="18" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
         <v>154</v>
       </c>
@@ -4156,7 +4315,7 @@
       <c r="M64" s="24"/>
       <c r="N64" s="24"/>
     </row>
-    <row r="65" spans="1:14" ht="18" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
         <v>143</v>
       </c>
@@ -4190,7 +4349,7 @@
       <c r="M65" s="24"/>
       <c r="N65" s="24"/>
     </row>
-    <row r="66" spans="1:14" ht="18" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
         <v>143</v>
       </c>
@@ -4224,7 +4383,7 @@
       <c r="M66" s="24"/>
       <c r="N66" s="24"/>
     </row>
-    <row r="67" spans="1:14" ht="18" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
         <v>143</v>
       </c>
@@ -4258,7 +4417,7 @@
       <c r="M67" s="24"/>
       <c r="N67" s="24"/>
     </row>
-    <row r="68" spans="1:14" ht="18" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
         <v>143</v>
       </c>
@@ -4300,7 +4459,7 @@
       </c>
       <c r="N68" s="24"/>
     </row>
-    <row r="69" spans="1:14" ht="18" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
         <v>154</v>
       </c>
@@ -4342,7 +4501,7 @@
       </c>
       <c r="N69" s="24"/>
     </row>
-    <row r="70" spans="1:14" ht="18" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
         <v>186</v>
       </c>
@@ -4382,7 +4541,7 @@
       </c>
       <c r="N70" s="24"/>
     </row>
-    <row r="71" spans="1:14" ht="18" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
         <v>193</v>
       </c>
@@ -4424,7 +4583,7 @@
       </c>
       <c r="N71" s="24"/>
     </row>
-    <row r="72" spans="1:14" ht="18" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
         <v>186</v>
       </c>
@@ -4466,7 +4625,7 @@
       </c>
       <c r="N72" s="24"/>
     </row>
-    <row r="73" spans="1:14" ht="18" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
         <v>193</v>
       </c>
@@ -4508,7 +4667,7 @@
       </c>
       <c r="N73" s="24"/>
     </row>
-    <row r="74" spans="1:14" ht="18" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
         <v>143</v>
       </c>
@@ -4542,7 +4701,7 @@
       <c r="M74" s="24"/>
       <c r="N74" s="24"/>
     </row>
-    <row r="75" spans="1:14" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A75" s="7" t="s">
         <v>143</v>
       </c>
@@ -4574,7 +4733,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="76" spans="1:14" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A76" s="7" t="s">
         <v>154</v>
       </c>
@@ -4612,7 +4771,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="77" spans="1:14" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A77" s="7" t="s">
         <v>193</v>
       </c>
@@ -4638,7 +4797,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="78" spans="1:14" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A78" s="7" t="s">
         <v>193</v>
       </c>
@@ -4664,7 +4823,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="79" spans="1:14" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A79" s="7" t="s">
         <v>193</v>
       </c>
@@ -4699,7 +4858,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="80" spans="1:14" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A80" s="7" t="s">
         <v>193</v>
       </c>
@@ -4728,7 +4887,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A81" s="7" t="s">
         <v>193</v>
       </c>
@@ -4757,7 +4916,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="82" spans="1:10" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A82" s="7" t="s">
         <v>193</v>
       </c>
@@ -4783,7 +4942,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="83" spans="1:10" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A83" s="30" t="s">
         <v>143</v>
       </c>
@@ -4809,7 +4968,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="84" spans="1:10" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A84" s="7" t="s">
         <v>193</v>
       </c>
@@ -4838,7 +4997,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="85" spans="1:10" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A85" s="7" t="s">
         <v>193</v>
       </c>
@@ -4867,7 +5026,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="86" spans="1:10" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A86" s="30" t="s">
         <v>186</v>
       </c>
@@ -4893,7 +5052,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="87" spans="1:10" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A87" s="7" t="s">
         <v>193</v>
       </c>

</xml_diff>

<commit_message>
Updated Read me COMS, and tests in Requirements documents
Added CF to list of tags

Added tests for sub systems
</commit_message>
<xml_diff>
--- a/requirements_design/HCS_Requirements_Documentation.xlsx
+++ b/requirements_design/HCS_Requirements_Documentation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7975897b035f41c7/my_files/UVIC/ROCKETRY/UVicRocketry_GITHUB/Hybrid-Controls-System/requirements_design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="276" documentId="11_F25DC773A252ABDACC104806C9D97FB05ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0F9BCE3C-3BA3-4456-A18C-A359E9D6A1CA}"/>
+  <xr:revisionPtr revIDLastSave="314" documentId="11_F25DC773A252ABDACC104806C9D97FB05ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{80B55011-506E-40FF-BDEE-F015309552E4}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="4395" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="System" sheetId="1" r:id="rId1"/>
@@ -20,10 +20,20 @@
     <sheet name="Valve Control Arduino" sheetId="5" r:id="rId5"/>
     <sheet name="EXAMPLE (FOR REFERENCE)" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -48,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="313">
   <si>
     <t>Date Changed</t>
   </si>
@@ -1216,6 +1226,53 @@
   </si>
   <si>
     <t>This communication line uses a fiber optic cable and two ethernet-fiber optic nodes</t>
+  </si>
+  <si>
+    <t>As the User, when I change the control switches states, the MCC should be aware of the change</t>
+  </si>
+  <si>
+    <t>Currently the states of the pins is constantly sent to the MCC which satisfies this requirement</t>
+  </si>
+  <si>
+    <t>MCC, CB</t>
+  </si>
+  <si>
+    <t>Updating control states</t>
+  </si>
+  <si>
+    <t>Systematically change the control state to a variety of combination</t>
+  </si>
+  <si>
+    <t>Control Box Assembled</t>
+  </si>
+  <si>
+    <t>Connect CB to computer or serial monitor
+Insure serial steam is being sent and read.
+Change all switches and observe results</t>
+  </si>
+  <si>
+    <t>Serial stream should change to reflect change in control box</t>
+  </si>
+  <si>
+    <t>Receive CB coms</t>
+  </si>
+  <si>
+    <t>Send and change serail information from CB to MCC. Insure the MCC can read the changing CB data</t>
+  </si>
+  <si>
+    <t>The MCC should read the CB data and update in 'real-time'</t>
+  </si>
+  <si>
+    <t>Serial output stream reflected changes to CB</t>
+  </si>
+  <si>
+    <t>Read Data</t>
+  </si>
+  <si>
+    <t>Read Data from the MCC sent from the CB</t>
+  </si>
+  <si>
+    <t>Connect the CB and MCC, Output data from the CB. Read the data through the MCC to the R-PI. Display the RPI data on a monitor. Change the CB inputs and observe the change</t>
   </si>
 </sst>
 </file>
@@ -1533,7 +1590,46 @@
     <cellStyle name="Heading 2" xfId="2" builtinId="17"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="45">
+  <dxfs count="58">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1785,99 +1881,97 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{F8107C66-607B-4058-88D5-7E54DAB777F3}" name="Table112" displayName="Table112" ref="C3:D20" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{F8107C66-607B-4058-88D5-7E54DAB777F3}" name="Table112" displayName="Table112" ref="C3:D20" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
   <autoFilter ref="C3:D20" xr:uid="{F8107C66-607B-4058-88D5-7E54DAB777F3}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{3CB6871F-D1D5-406A-A5F6-6C3D55F08377}" name="R#" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{4EAFD1C8-470F-415F-8511-C74AAEBC13D5}" name="Requirement" dataDxfId="17"/>
+    <tableColumn id="1" xr3:uid="{3CB6871F-D1D5-406A-A5F6-6C3D55F08377}" name="R#" dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{4EAFD1C8-470F-415F-8511-C74AAEBC13D5}" name="Requirement" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{3ABBEBA9-0A73-4764-B21E-B89DEA853C72}" name="Table213" displayName="Table213" ref="A61:N88" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15" headerRowCellStyle="Heading 1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{3ABBEBA9-0A73-4764-B21E-B89DEA853C72}" name="Table213" displayName="Table213" ref="A61:N88" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" headerRowCellStyle="Heading 1">
   <autoFilter ref="A61:N88" xr:uid="{3ABBEBA9-0A73-4764-B21E-B89DEA853C72}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A62:N104">
     <sortCondition ref="B1:B44"/>
   </sortState>
   <tableColumns count="14">
-    <tableColumn id="13" xr3:uid="{F3FFF02B-2482-42E9-B584-8F4D96166CA9}" name="Test Suite" dataDxfId="13"/>
-    <tableColumn id="11" xr3:uid="{1FB81E90-5ADA-4A56-88E3-E9B7D133719D}" name="Test Case No." dataDxfId="12"/>
-    <tableColumn id="1" xr3:uid="{0241E09D-793F-44A7-B410-7D90C214292F}" name="R No." dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{C02C19C0-E85F-4B0D-9246-CEF8EEF91981}" name="Scenario No." dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{D06ABCE0-F28E-4D7C-A949-E93075902232}" name="Test Decription" dataDxfId="9"/>
-    <tableColumn id="14" xr3:uid="{25B688DF-563E-4077-9340-7112817C8A39}" name="Interface" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{065BAE68-A3D8-4003-AD54-4BFAFFAE8D78}" name="Pre-requisites" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{0F72F42F-2308-4A45-A9BB-DA60FBC6FE2C}" name="Test Steps" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{3DF66932-C56F-4194-BF09-A7E4A2C41CC5}" name="Test Data" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{B8964114-923E-4588-A3C3-4C6FD4E8B523}" name="Expected Results" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{D3CA6EED-7389-48FF-A0B4-A7012E5844C3}" name="Actual Results" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{BE9DFA11-ED6D-4049-A2E2-267CB763A2C8}" name="Post Conditions" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{E0BDA9F2-509F-4DA0-9845-C87731E235F2}" name="Pass/Fail" dataDxfId="1"/>
-    <tableColumn id="12" xr3:uid="{C0F69B75-B8DE-4212-944C-F980F5FE35FB}" name="Comments" dataDxfId="0"/>
+    <tableColumn id="13" xr3:uid="{F3FFF02B-2482-42E9-B584-8F4D96166CA9}" name="Test Suite" dataDxfId="26"/>
+    <tableColumn id="11" xr3:uid="{1FB81E90-5ADA-4A56-88E3-E9B7D133719D}" name="Test Case No." dataDxfId="25"/>
+    <tableColumn id="1" xr3:uid="{0241E09D-793F-44A7-B410-7D90C214292F}" name="R No." dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{C02C19C0-E85F-4B0D-9246-CEF8EEF91981}" name="Scenario No." dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{D06ABCE0-F28E-4D7C-A949-E93075902232}" name="Test Decription" dataDxfId="22"/>
+    <tableColumn id="14" xr3:uid="{25B688DF-563E-4077-9340-7112817C8A39}" name="Interface" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{065BAE68-A3D8-4003-AD54-4BFAFFAE8D78}" name="Pre-requisites" dataDxfId="20"/>
+    <tableColumn id="6" xr3:uid="{0F72F42F-2308-4A45-A9BB-DA60FBC6FE2C}" name="Test Steps" dataDxfId="19"/>
+    <tableColumn id="7" xr3:uid="{3DF66932-C56F-4194-BF09-A7E4A2C41CC5}" name="Test Data" dataDxfId="18"/>
+    <tableColumn id="8" xr3:uid="{B8964114-923E-4588-A3C3-4C6FD4E8B523}" name="Expected Results" dataDxfId="17"/>
+    <tableColumn id="9" xr3:uid="{D3CA6EED-7389-48FF-A0B4-A7012E5844C3}" name="Actual Results" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{BE9DFA11-ED6D-4049-A2E2-267CB763A2C8}" name="Post Conditions" dataDxfId="15"/>
+    <tableColumn id="10" xr3:uid="{E0BDA9F2-509F-4DA0-9845-C87731E235F2}" name="Pass/Fail" dataDxfId="14"/>
+    <tableColumn id="12" xr3:uid="{C0F69B75-B8DE-4212-944C-F980F5FE35FB}" name="Comments" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5FA4E805-D57D-4D43-9E0B-5E331A6D663E}" name="Table14" displayName="Table14" ref="D11:H30" totalsRowShown="0" dataDxfId="44" headerRowCellStyle="Heading 2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5FA4E805-D57D-4D43-9E0B-5E331A6D663E}" name="Table14" displayName="Table14" ref="D11:H30" totalsRowShown="0" dataDxfId="57" headerRowCellStyle="Heading 2">
   <autoFilter ref="D11:H30" xr:uid="{5FA4E805-D57D-4D43-9E0B-5E331A6D663E}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{BB1AF20A-CAB4-4CAB-81A5-CCAF14E79FE3}" name="Requirements" dataDxfId="43"/>
-    <tableColumn id="2" xr3:uid="{4DDE8730-E55A-4A81-BB34-A3E37063B965}" name="Description" dataDxfId="42"/>
-    <tableColumn id="3" xr3:uid="{F3723AD1-E0EE-4DAC-9210-7176FAFCDB41}" name="User Stories/Scenarios" dataDxfId="41"/>
-    <tableColumn id="4" xr3:uid="{7DE1817D-340D-4D60-8755-7170363B6042}" name="Notes" dataDxfId="40"/>
-    <tableColumn id="5" xr3:uid="{98DCC91C-BCC8-4706-B1E4-66C4499EBEB7}" name="Affected Systems" dataDxfId="39"/>
+    <tableColumn id="1" xr3:uid="{BB1AF20A-CAB4-4CAB-81A5-CCAF14E79FE3}" name="Requirements" dataDxfId="56"/>
+    <tableColumn id="2" xr3:uid="{4DDE8730-E55A-4A81-BB34-A3E37063B965}" name="Description" dataDxfId="55"/>
+    <tableColumn id="3" xr3:uid="{F3723AD1-E0EE-4DAC-9210-7176FAFCDB41}" name="User Stories/Scenarios" dataDxfId="54"/>
+    <tableColumn id="4" xr3:uid="{7DE1817D-340D-4D60-8755-7170363B6042}" name="Notes" dataDxfId="53"/>
+    <tableColumn id="5" xr3:uid="{98DCC91C-BCC8-4706-B1E4-66C4499EBEB7}" name="Affected Systems" dataDxfId="52"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E72C23B9-2964-4B53-98EE-7AF6DA61F8CA}" name="Table25" displayName="Table25" ref="D39:P59" totalsRowShown="0" headerRowCellStyle="Heading 2">
-  <autoFilter ref="D39:P59" xr:uid="{E72C23B9-2964-4B53-98EE-7AF6DA61F8CA}"/>
-  <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{72046022-7EAC-4631-B8FE-B78DB2E83429}" name="Test Cases"/>
-    <tableColumn id="2" xr3:uid="{577F2597-19D1-49F7-A8A4-8DBEA782ADED}" name="R No."/>
-    <tableColumn id="3" xr3:uid="{1D5177EE-3B6D-4EE1-BB01-996DD17BFF52}" name="Scenario No."/>
-    <tableColumn id="4" xr3:uid="{E754B080-ED6A-4DDD-8B73-463673C991D6}" name="Test Decription"/>
-    <tableColumn id="5" xr3:uid="{4C354F30-C87D-465B-A19C-FAAB26079169}" name="Interface"/>
-    <tableColumn id="6" xr3:uid="{C20DB11E-A7A6-48E6-88C4-D152DF7DED61}" name="Pre-requisites"/>
-    <tableColumn id="7" xr3:uid="{F4C85738-0BC3-472A-9E9A-0E55DF17D864}" name="Test Steps"/>
-    <tableColumn id="8" xr3:uid="{3AAA83DE-C90A-45B6-9C1F-AD1BC81653A4}" name="Test Data"/>
-    <tableColumn id="9" xr3:uid="{B774C0FD-EFC7-4B75-B3AC-2F34FD56BB42}" name="Expected Results"/>
-    <tableColumn id="10" xr3:uid="{BD7B262C-507F-4F8D-99F7-3890A7B60ED1}" name="Actual Results"/>
-    <tableColumn id="11" xr3:uid="{7EA8F3BB-1310-41AF-AF6A-95AC583883FE}" name="Post Conditions"/>
-    <tableColumn id="12" xr3:uid="{D1247FE9-8C34-48CE-9EA4-66D2C4C6FA94}" name="Pass/Fail"/>
-    <tableColumn id="13" xr3:uid="{61696DBC-80A8-4BAB-936B-D0C672C87DFB}" name="Comments"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E72C23B9-2964-4B53-98EE-7AF6DA61F8CA}" name="Table25" displayName="Table25" ref="D39:O59" totalsRowShown="0" dataDxfId="0" headerRowCellStyle="Heading 2">
+  <autoFilter ref="D39:O59" xr:uid="{E72C23B9-2964-4B53-98EE-7AF6DA61F8CA}"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{72046022-7EAC-4631-B8FE-B78DB2E83429}" name="Test Cases" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{577F2597-19D1-49F7-A8A4-8DBEA782ADED}" name="R No." dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{1D5177EE-3B6D-4EE1-BB01-996DD17BFF52}" name="Scenario No." dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{E754B080-ED6A-4DDD-8B73-463673C991D6}" name="Test Decription" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{C20DB11E-A7A6-48E6-88C4-D152DF7DED61}" name="Pre-requisites" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{F4C85738-0BC3-472A-9E9A-0E55DF17D864}" name="Test Steps" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{3AAA83DE-C90A-45B6-9C1F-AD1BC81653A4}" name="Test Data" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{B774C0FD-EFC7-4B75-B3AC-2F34FD56BB42}" name="Expected Results" dataDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{BD7B262C-507F-4F8D-99F7-3890A7B60ED1}" name="Actual Results" dataDxfId="4"/>
+    <tableColumn id="11" xr3:uid="{7EA8F3BB-1310-41AF-AF6A-95AC583883FE}" name="Post Conditions" dataDxfId="3"/>
+    <tableColumn id="12" xr3:uid="{D1247FE9-8C34-48CE-9EA4-66D2C4C6FA94}" name="Pass/Fail" dataDxfId="2"/>
+    <tableColumn id="13" xr3:uid="{61696DBC-80A8-4BAB-936B-D0C672C87DFB}" name="Comments" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{90DF5E57-F0F7-4FA0-8DE8-33E1F966054E}" name="Table16" displayName="Table16" ref="D11:H30" totalsRowShown="0" dataDxfId="38" headerRowCellStyle="Heading 2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{90DF5E57-F0F7-4FA0-8DE8-33E1F966054E}" name="Table16" displayName="Table16" ref="D11:H30" totalsRowShown="0" dataDxfId="51" headerRowCellStyle="Heading 2">
   <autoFilter ref="D11:H30" xr:uid="{90DF5E57-F0F7-4FA0-8DE8-33E1F966054E}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{46746041-5C2F-4000-B825-78DCEE5C7F5D}" name="Requirements" dataDxfId="37"/>
-    <tableColumn id="2" xr3:uid="{A2917C86-AE50-404F-B2E2-45D77DB803DB}" name="Description" dataDxfId="36"/>
-    <tableColumn id="3" xr3:uid="{5BDBE60B-9C74-440C-960D-6FF584AAF1CC}" name="User Stories/Scenarios" dataDxfId="35"/>
-    <tableColumn id="4" xr3:uid="{403A2FD3-FDB5-4EB3-881D-3777DE4FBE4E}" name="Notes" dataDxfId="34"/>
-    <tableColumn id="5" xr3:uid="{B1A66192-CECE-4C07-A94F-0B1DD4A33300}" name="Affected Systems" dataDxfId="33"/>
+    <tableColumn id="1" xr3:uid="{46746041-5C2F-4000-B825-78DCEE5C7F5D}" name="Requirements" dataDxfId="50"/>
+    <tableColumn id="2" xr3:uid="{A2917C86-AE50-404F-B2E2-45D77DB803DB}" name="Description" dataDxfId="49"/>
+    <tableColumn id="3" xr3:uid="{5BDBE60B-9C74-440C-960D-6FF584AAF1CC}" name="User Stories/Scenarios" dataDxfId="48"/>
+    <tableColumn id="4" xr3:uid="{403A2FD3-FDB5-4EB3-881D-3777DE4FBE4E}" name="Notes" dataDxfId="47"/>
+    <tableColumn id="5" xr3:uid="{B1A66192-CECE-4C07-A94F-0B1DD4A33300}" name="Affected Systems" dataDxfId="46"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{34380E41-180F-4ED1-96AD-C422C14E13A9}" name="Table27" displayName="Table27" ref="D39:P59" totalsRowShown="0" headerRowCellStyle="Heading 2">
-  <autoFilter ref="D39:P59" xr:uid="{34380E41-180F-4ED1-96AD-C422C14E13A9}"/>
-  <tableColumns count="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{34380E41-180F-4ED1-96AD-C422C14E13A9}" name="Table27" displayName="Table27" ref="D39:O59" totalsRowShown="0" headerRowCellStyle="Heading 2">
+  <autoFilter ref="D39:O59" xr:uid="{34380E41-180F-4ED1-96AD-C422C14E13A9}"/>
+  <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{BB57CFDD-8388-43CE-8424-290957997977}" name="Test Cases"/>
     <tableColumn id="2" xr3:uid="{E0D233C1-BC97-494F-A8C4-AF688CFF6896}" name="R No."/>
-    <tableColumn id="3" xr3:uid="{EDFA8644-B567-4B99-88EC-48023D120DB8}" name="Scenario No."/>
     <tableColumn id="4" xr3:uid="{4B668B27-11A6-42E0-A6FE-F787AF561B86}" name="Test Decription"/>
     <tableColumn id="5" xr3:uid="{3F225959-8A9C-4621-8495-2255F773CDF6}" name="Interface"/>
     <tableColumn id="6" xr3:uid="{3084F3B5-E831-4685-B3C7-50A3EF256247}" name="Pre-requisites"/>
@@ -1894,26 +1988,25 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{A611E60F-4F24-4EB3-8CDC-8BBB573550F0}" name="Table18" displayName="Table18" ref="D11:H30" totalsRowShown="0" dataDxfId="32" headerRowCellStyle="Heading 2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{A611E60F-4F24-4EB3-8CDC-8BBB573550F0}" name="Table18" displayName="Table18" ref="D11:H30" totalsRowShown="0" dataDxfId="45" headerRowCellStyle="Heading 2">
   <autoFilter ref="D11:H30" xr:uid="{A611E60F-4F24-4EB3-8CDC-8BBB573550F0}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{E7FF2F9A-AB1C-4193-B154-F0080371199F}" name="Requirements" dataDxfId="31"/>
-    <tableColumn id="2" xr3:uid="{05F92AD7-E08F-4A7B-8CD0-5AD6A6659F64}" name="Description" dataDxfId="30"/>
-    <tableColumn id="3" xr3:uid="{52E9F203-1862-4583-8088-FB60845FE8FF}" name="User Stories/Scenarios" dataDxfId="29"/>
-    <tableColumn id="4" xr3:uid="{319355A8-A488-4D7D-89B7-E25B1E3092E4}" name="Notes" dataDxfId="28"/>
-    <tableColumn id="5" xr3:uid="{84602B21-3F71-4BC1-A799-E4208D2D39A4}" name="Affected Systems" dataDxfId="27"/>
+    <tableColumn id="1" xr3:uid="{E7FF2F9A-AB1C-4193-B154-F0080371199F}" name="Requirements" dataDxfId="44"/>
+    <tableColumn id="2" xr3:uid="{05F92AD7-E08F-4A7B-8CD0-5AD6A6659F64}" name="Description" dataDxfId="43"/>
+    <tableColumn id="3" xr3:uid="{52E9F203-1862-4583-8088-FB60845FE8FF}" name="User Stories/Scenarios" dataDxfId="42"/>
+    <tableColumn id="4" xr3:uid="{319355A8-A488-4D7D-89B7-E25B1E3092E4}" name="Notes" dataDxfId="41"/>
+    <tableColumn id="5" xr3:uid="{84602B21-3F71-4BC1-A799-E4208D2D39A4}" name="Affected Systems" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{E54182DD-5242-46BD-81F7-57A1EC0A1412}" name="Table29" displayName="Table29" ref="D39:P59" totalsRowShown="0" headerRowCellStyle="Heading 2">
-  <autoFilter ref="D39:P59" xr:uid="{E54182DD-5242-46BD-81F7-57A1EC0A1412}"/>
-  <tableColumns count="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{E54182DD-5242-46BD-81F7-57A1EC0A1412}" name="Table29" displayName="Table29" ref="D39:O59" totalsRowShown="0" headerRowCellStyle="Heading 2">
+  <autoFilter ref="D39:O59" xr:uid="{E54182DD-5242-46BD-81F7-57A1EC0A1412}"/>
+  <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{EB6EDC21-AFCC-4658-9466-B229AFE6C048}" name="Test Cases"/>
     <tableColumn id="2" xr3:uid="{B28DDB53-47DB-4650-8EBC-76C560DC4A69}" name="R No."/>
-    <tableColumn id="3" xr3:uid="{159AD39A-5B75-4AD5-9658-D334C8F6824C}" name="Scenario No."/>
     <tableColumn id="4" xr3:uid="{FA8A0A46-CFFF-4F87-82C6-1DB85F4815B0}" name="Test Decription"/>
     <tableColumn id="5" xr3:uid="{1FD842BC-A613-42B6-B766-C929BB8CF961}" name="Interface"/>
     <tableColumn id="6" xr3:uid="{8DE1C65A-89CB-4CED-AFC8-6F41E8408BA2}" name="Pre-requisites"/>
@@ -1930,14 +2023,14 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{99C0BC7D-645F-4D4D-8BF0-B7A914E8F15D}" name="Table110" displayName="Table110" ref="D11:H30" totalsRowShown="0" dataDxfId="26" headerRowCellStyle="Heading 2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{99C0BC7D-645F-4D4D-8BF0-B7A914E8F15D}" name="Table110" displayName="Table110" ref="D11:H30" totalsRowShown="0" dataDxfId="39" headerRowCellStyle="Heading 2">
   <autoFilter ref="D11:H30" xr:uid="{99C0BC7D-645F-4D4D-8BF0-B7A914E8F15D}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{246CB3CD-654F-4B86-AF12-B19A107142F8}" name="Requirements" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{663BD34F-A7D9-450A-920D-FE75EDE33F04}" name="Description" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{9DBD0301-DDD7-471D-B108-491ADD7E6356}" name="User Stories/Scenarios" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{904A52D0-E01F-4764-9605-DF8BAB3F1860}" name="Notes" dataDxfId="22"/>
-    <tableColumn id="5" xr3:uid="{139A7663-409F-4E01-AE76-E84F213827DF}" name="Affected Systems" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{246CB3CD-654F-4B86-AF12-B19A107142F8}" name="Requirements" dataDxfId="38"/>
+    <tableColumn id="2" xr3:uid="{663BD34F-A7D9-450A-920D-FE75EDE33F04}" name="Description" dataDxfId="37"/>
+    <tableColumn id="3" xr3:uid="{9DBD0301-DDD7-471D-B108-491ADD7E6356}" name="User Stories/Scenarios" dataDxfId="36"/>
+    <tableColumn id="4" xr3:uid="{904A52D0-E01F-4764-9605-DF8BAB3F1860}" name="Notes" dataDxfId="35"/>
+    <tableColumn id="5" xr3:uid="{139A7663-409F-4E01-AE76-E84F213827DF}" name="Affected Systems" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2238,31 +2331,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C16" workbookViewId="0">
+    <sheetView topLeftCell="C16" workbookViewId="0">
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" customWidth="1"/>
-    <col min="2" max="2" width="36.7109375" customWidth="1"/>
-    <col min="3" max="3" width="45.5703125" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" customWidth="1"/>
-    <col min="5" max="5" width="68.42578125" customWidth="1"/>
-    <col min="6" max="6" width="60.28515625" customWidth="1"/>
+    <col min="1" max="1" width="21.86328125" customWidth="1"/>
+    <col min="2" max="2" width="36.73046875" customWidth="1"/>
+    <col min="3" max="3" width="45.59765625" customWidth="1"/>
+    <col min="4" max="4" width="20.1328125" customWidth="1"/>
+    <col min="5" max="5" width="68.3984375" customWidth="1"/>
+    <col min="6" max="6" width="60.265625" customWidth="1"/>
     <col min="7" max="7" width="34" customWidth="1"/>
-    <col min="8" max="8" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.3984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.86328125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.1328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.1328125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="18" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.3984375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2273,7 +2366,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2284,7 +2377,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2292,12 +2385,12 @@
         <v>267</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="D11" s="1" t="s">
         <v>5</v>
       </c>
@@ -2314,7 +2407,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="43.15" thickTop="1" x14ac:dyDescent="0.45">
       <c r="D12" s="5">
         <v>1</v>
       </c>
@@ -2329,7 +2422,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="D13" s="5">
         <v>2</v>
       </c>
@@ -2342,7 +2435,7 @@
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D14" s="5">
         <v>3</v>
       </c>
@@ -2355,7 +2448,7 @@
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="D15" s="5">
         <v>4</v>
       </c>
@@ -2368,7 +2461,7 @@
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D16" s="5">
         <v>5</v>
       </c>
@@ -2379,7 +2472,7 @@
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="D17" s="5">
         <v>6</v>
       </c>
@@ -2390,28 +2483,28 @@
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A21" s="32" t="s">
         <v>297</v>
       </c>
@@ -2421,64 +2514,64 @@
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
     </row>
-    <row r="39" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="40" spans="3:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="40" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C40" s="31" t="s">
         <v>294</v>
       </c>
@@ -2492,7 +2585,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="41" spans="3:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:6" ht="31.15" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C41" s="31" t="s">
         <v>273</v>
       </c>
@@ -2506,7 +2599,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="42" spans="3:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:6" ht="31.15" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C42" s="31" t="s">
         <v>276</v>
       </c>
@@ -2520,7 +2613,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="43" spans="3:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:6" ht="31.15" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C43" s="31" t="s">
         <v>279</v>
       </c>
@@ -2534,7 +2627,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="44" spans="3:6" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:6" ht="46.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C44" s="31" t="s">
         <v>282</v>
       </c>
@@ -2548,7 +2641,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="45" spans="3:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:6" ht="31.15" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C45" s="31" t="s">
         <v>285</v>
       </c>
@@ -2562,7 +2655,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="46" spans="3:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C46" s="31" t="s">
         <v>288</v>
       </c>
@@ -2576,7 +2669,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="47" spans="3:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C47" s="31" t="s">
         <v>291</v>
       </c>
@@ -2601,32 +2694,32 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD2CFAC1-75F2-45AC-BC39-20C1FFB4D1E2}">
-  <dimension ref="A1:P40"/>
+  <dimension ref="A1:O59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B3"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="2" max="2" width="34.5703125" customWidth="1"/>
-    <col min="3" max="3" width="36.85546875" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.3984375" customWidth="1"/>
+    <col min="2" max="2" width="34.59765625" customWidth="1"/>
+    <col min="3" max="3" width="36.86328125" customWidth="1"/>
+    <col min="4" max="4" width="20.59765625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="53" customWidth="1"/>
-    <col min="6" max="6" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.86328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="54.86328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.3984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.86328125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="48.3984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="36.1328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="21.06640625" customWidth="1"/>
+    <col min="15" max="15" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2637,7 +2730,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2645,7 +2738,7 @@
         <v>44691</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2653,12 +2746,12 @@
         <v>267</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="D11" s="1" t="s">
         <v>5</v>
       </c>
@@ -2675,7 +2768,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="28.9" thickTop="1" x14ac:dyDescent="0.45">
       <c r="D12" s="5">
         <v>1</v>
       </c>
@@ -2686,7 +2779,7 @@
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
     </row>
-    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="D13" s="5">
         <v>2</v>
       </c>
@@ -2697,18 +2790,24 @@
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
       <c r="D14" s="5">
         <v>3</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-    </row>
-    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="F14" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="D15" s="5">
         <v>4</v>
       </c>
@@ -2719,7 +2818,7 @@
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="D16" s="5">
         <v>5</v>
       </c>
@@ -2730,7 +2829,7 @@
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="4:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="D17" s="5">
         <v>6</v>
       </c>
@@ -2741,98 +2840,98 @@
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
     </row>
-    <row r="18" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
     </row>
-    <row r="19" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
     </row>
-    <row r="20" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
     </row>
-    <row r="21" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
     </row>
-    <row r="22" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
     </row>
-    <row r="23" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
     </row>
-    <row r="24" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
     </row>
-    <row r="25" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
     </row>
-    <row r="26" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
     </row>
-    <row r="27" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
     </row>
-    <row r="28" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
     </row>
-    <row r="29" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
     </row>
-    <row r="30" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
     </row>
-    <row r="39" spans="4:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="4:15" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="D39" s="1" t="s">
         <v>10</v>
       </c>
@@ -2846,34 +2945,324 @@
         <v>13</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M39" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N39" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O39" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="P39" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="4:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="4:15" ht="57.4" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="D40" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="E40" s="5">
+        <v>3</v>
+      </c>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="I40" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="J40" s="5"/>
+      <c r="K40" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="L40" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="M40" s="5"/>
+      <c r="N40" s="5"/>
+      <c r="O40" s="5"/>
+    </row>
+    <row r="41" spans="4:15" x14ac:dyDescent="0.45">
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
+      <c r="I41" s="5"/>
+      <c r="J41" s="5"/>
+      <c r="K41" s="5"/>
+      <c r="L41" s="5"/>
+      <c r="M41" s="5"/>
+      <c r="N41" s="5"/>
+      <c r="O41" s="5"/>
+    </row>
+    <row r="42" spans="4:15" x14ac:dyDescent="0.45">
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="5"/>
+      <c r="I42" s="5"/>
+      <c r="J42" s="5"/>
+      <c r="K42" s="5"/>
+      <c r="L42" s="5"/>
+      <c r="M42" s="5"/>
+      <c r="N42" s="5"/>
+      <c r="O42" s="5"/>
+    </row>
+    <row r="43" spans="4:15" x14ac:dyDescent="0.45">
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="5"/>
+      <c r="H43" s="5"/>
+      <c r="I43" s="5"/>
+      <c r="J43" s="5"/>
+      <c r="K43" s="5"/>
+      <c r="L43" s="5"/>
+      <c r="M43" s="5"/>
+      <c r="N43" s="5"/>
+      <c r="O43" s="5"/>
+    </row>
+    <row r="44" spans="4:15" x14ac:dyDescent="0.45">
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="5"/>
+      <c r="H44" s="5"/>
+      <c r="I44" s="5"/>
+      <c r="J44" s="5"/>
+      <c r="K44" s="5"/>
+      <c r="L44" s="5"/>
+      <c r="M44" s="5"/>
+      <c r="N44" s="5"/>
+      <c r="O44" s="5"/>
+    </row>
+    <row r="45" spans="4:15" x14ac:dyDescent="0.45">
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
+      <c r="I45" s="5"/>
+      <c r="J45" s="5"/>
+      <c r="K45" s="5"/>
+      <c r="L45" s="5"/>
+      <c r="M45" s="5"/>
+      <c r="N45" s="5"/>
+      <c r="O45" s="5"/>
+    </row>
+    <row r="46" spans="4:15" x14ac:dyDescent="0.45">
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="5"/>
+      <c r="H46" s="5"/>
+      <c r="I46" s="5"/>
+      <c r="J46" s="5"/>
+      <c r="K46" s="5"/>
+      <c r="L46" s="5"/>
+      <c r="M46" s="5"/>
+      <c r="N46" s="5"/>
+      <c r="O46" s="5"/>
+    </row>
+    <row r="47" spans="4:15" x14ac:dyDescent="0.45">
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
+      <c r="H47" s="5"/>
+      <c r="I47" s="5"/>
+      <c r="J47" s="5"/>
+      <c r="K47" s="5"/>
+      <c r="L47" s="5"/>
+      <c r="M47" s="5"/>
+      <c r="N47" s="5"/>
+      <c r="O47" s="5"/>
+    </row>
+    <row r="48" spans="4:15" x14ac:dyDescent="0.45">
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="5"/>
+      <c r="H48" s="5"/>
+      <c r="I48" s="5"/>
+      <c r="J48" s="5"/>
+      <c r="K48" s="5"/>
+      <c r="L48" s="5"/>
+      <c r="M48" s="5"/>
+      <c r="N48" s="5"/>
+      <c r="O48" s="5"/>
+    </row>
+    <row r="49" spans="4:15" x14ac:dyDescent="0.45">
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="5"/>
+      <c r="H49" s="5"/>
+      <c r="I49" s="5"/>
+      <c r="J49" s="5"/>
+      <c r="K49" s="5"/>
+      <c r="L49" s="5"/>
+      <c r="M49" s="5"/>
+      <c r="N49" s="5"/>
+      <c r="O49" s="5"/>
+    </row>
+    <row r="50" spans="4:15" x14ac:dyDescent="0.45">
+      <c r="D50" s="5"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="5"/>
+      <c r="G50" s="5"/>
+      <c r="H50" s="5"/>
+      <c r="I50" s="5"/>
+      <c r="J50" s="5"/>
+      <c r="K50" s="5"/>
+      <c r="L50" s="5"/>
+      <c r="M50" s="5"/>
+      <c r="N50" s="5"/>
+      <c r="O50" s="5"/>
+    </row>
+    <row r="51" spans="4:15" x14ac:dyDescent="0.45">
+      <c r="D51" s="5"/>
+      <c r="E51" s="5"/>
+      <c r="F51" s="5"/>
+      <c r="G51" s="5"/>
+      <c r="H51" s="5"/>
+      <c r="I51" s="5"/>
+      <c r="J51" s="5"/>
+      <c r="K51" s="5"/>
+      <c r="L51" s="5"/>
+      <c r="M51" s="5"/>
+      <c r="N51" s="5"/>
+      <c r="O51" s="5"/>
+    </row>
+    <row r="52" spans="4:15" x14ac:dyDescent="0.45">
+      <c r="D52" s="5"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="5"/>
+      <c r="G52" s="5"/>
+      <c r="H52" s="5"/>
+      <c r="I52" s="5"/>
+      <c r="J52" s="5"/>
+      <c r="K52" s="5"/>
+      <c r="L52" s="5"/>
+      <c r="M52" s="5"/>
+      <c r="N52" s="5"/>
+      <c r="O52" s="5"/>
+    </row>
+    <row r="53" spans="4:15" x14ac:dyDescent="0.45">
+      <c r="D53" s="5"/>
+      <c r="E53" s="5"/>
+      <c r="F53" s="5"/>
+      <c r="G53" s="5"/>
+      <c r="H53" s="5"/>
+      <c r="I53" s="5"/>
+      <c r="J53" s="5"/>
+      <c r="K53" s="5"/>
+      <c r="L53" s="5"/>
+      <c r="M53" s="5"/>
+      <c r="N53" s="5"/>
+      <c r="O53" s="5"/>
+    </row>
+    <row r="54" spans="4:15" x14ac:dyDescent="0.45">
+      <c r="D54" s="5"/>
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
+      <c r="G54" s="5"/>
+      <c r="H54" s="5"/>
+      <c r="I54" s="5"/>
+      <c r="J54" s="5"/>
+      <c r="K54" s="5"/>
+      <c r="L54" s="5"/>
+      <c r="M54" s="5"/>
+      <c r="N54" s="5"/>
+      <c r="O54" s="5"/>
+    </row>
+    <row r="55" spans="4:15" x14ac:dyDescent="0.45">
+      <c r="D55" s="5"/>
+      <c r="E55" s="5"/>
+      <c r="F55" s="5"/>
+      <c r="G55" s="5"/>
+      <c r="H55" s="5"/>
+      <c r="I55" s="5"/>
+      <c r="J55" s="5"/>
+      <c r="K55" s="5"/>
+      <c r="L55" s="5"/>
+      <c r="M55" s="5"/>
+      <c r="N55" s="5"/>
+      <c r="O55" s="5"/>
+    </row>
+    <row r="56" spans="4:15" x14ac:dyDescent="0.45">
+      <c r="D56" s="5"/>
+      <c r="E56" s="5"/>
+      <c r="F56" s="5"/>
+      <c r="G56" s="5"/>
+      <c r="H56" s="5"/>
+      <c r="I56" s="5"/>
+      <c r="J56" s="5"/>
+      <c r="K56" s="5"/>
+      <c r="L56" s="5"/>
+      <c r="M56" s="5"/>
+      <c r="N56" s="5"/>
+      <c r="O56" s="5"/>
+    </row>
+    <row r="57" spans="4:15" x14ac:dyDescent="0.45">
+      <c r="D57" s="5"/>
+      <c r="E57" s="5"/>
+      <c r="F57" s="5"/>
+      <c r="G57" s="5"/>
+      <c r="H57" s="5"/>
+      <c r="I57" s="5"/>
+      <c r="J57" s="5"/>
+      <c r="K57" s="5"/>
+      <c r="L57" s="5"/>
+      <c r="M57" s="5"/>
+      <c r="N57" s="5"/>
+      <c r="O57" s="5"/>
+    </row>
+    <row r="58" spans="4:15" x14ac:dyDescent="0.45">
+      <c r="D58" s="5"/>
+      <c r="E58" s="5"/>
+      <c r="F58" s="5"/>
+      <c r="G58" s="5"/>
+      <c r="H58" s="5"/>
+      <c r="I58" s="5"/>
+      <c r="J58" s="5"/>
+      <c r="K58" s="5"/>
+      <c r="L58" s="5"/>
+      <c r="M58" s="5"/>
+      <c r="N58" s="5"/>
+      <c r="O58" s="5"/>
+    </row>
+    <row r="59" spans="4:15" x14ac:dyDescent="0.45">
+      <c r="D59" s="5"/>
+      <c r="E59" s="5"/>
+      <c r="F59" s="5"/>
+      <c r="G59" s="5"/>
+      <c r="H59" s="5"/>
+      <c r="I59" s="5"/>
+      <c r="J59" s="5"/>
+      <c r="K59" s="5"/>
+      <c r="L59" s="5"/>
+      <c r="M59" s="5"/>
+      <c r="N59" s="5"/>
+      <c r="O59" s="5"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="2">
@@ -2885,33 +3274,33 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87C15626-044F-4C0A-A2A5-E60D99F36C59}">
-  <dimension ref="A1:P40"/>
+  <dimension ref="A1:O40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B3"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" customWidth="1"/>
+    <col min="1" max="1" width="27.73046875" customWidth="1"/>
+    <col min="2" max="2" width="24.73046875" customWidth="1"/>
     <col min="3" max="3" width="44" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="63.5703125" customWidth="1"/>
-    <col min="6" max="6" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.59765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="63.59765625" customWidth="1"/>
+    <col min="6" max="6" width="79.9296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.1328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.3984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.86328125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="48.86328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.1328125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="18" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.3984375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.53125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2922,7 +3311,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2930,7 +3319,7 @@
         <v>44691</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2938,12 +3327,12 @@
         <v>267</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="D11" s="1" t="s">
         <v>5</v>
       </c>
@@ -2960,7 +3349,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="28.9" thickTop="1" x14ac:dyDescent="0.45">
       <c r="D12" s="5">
         <v>1</v>
       </c>
@@ -2971,7 +3360,7 @@
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D13" s="5">
         <v>2</v>
       </c>
@@ -2982,7 +3371,7 @@
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D14" s="5">
         <v>3</v>
       </c>
@@ -2993,7 +3382,7 @@
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="D15" s="5">
         <v>4</v>
       </c>
@@ -3004,7 +3393,7 @@
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="D16" s="5">
         <v>5</v>
       </c>
@@ -3015,105 +3404,105 @@
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
     </row>
-    <row r="18" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
     </row>
-    <row r="19" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
     </row>
-    <row r="20" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
     </row>
-    <row r="21" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
     </row>
-    <row r="22" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
     </row>
-    <row r="23" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
     </row>
-    <row r="24" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
     </row>
-    <row r="25" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
     </row>
-    <row r="26" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
     </row>
-    <row r="27" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
     </row>
-    <row r="28" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
     </row>
-    <row r="29" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
     </row>
-    <row r="30" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
     </row>
-    <row r="39" spans="4:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="4:15" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="D39" s="1" t="s">
         <v>10</v>
       </c>
@@ -3121,40 +3510,50 @@
         <v>11</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M39" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N39" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O39" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="P39" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="4:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="4:15" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="D40" t="s">
+        <v>306</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40" t="s">
+        <v>307</v>
+      </c>
+      <c r="K40" t="s">
+        <v>308</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="2">
@@ -3166,31 +3565,31 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDABCBC9-6A47-47E2-A95B-2A3FC972965A}">
-  <dimension ref="A1:P40"/>
+  <dimension ref="A1:O40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="E19" workbookViewId="0">
+      <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" customWidth="1"/>
-    <col min="2" max="2" width="49.5703125" customWidth="1"/>
-    <col min="4" max="4" width="40.5703125" customWidth="1"/>
-    <col min="5" max="5" width="75.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.28515625" customWidth="1"/>
+    <col min="1" max="1" width="30.265625" customWidth="1"/>
+    <col min="2" max="2" width="49.59765625" customWidth="1"/>
+    <col min="4" max="4" width="40.59765625" customWidth="1"/>
+    <col min="5" max="5" width="75.59765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.265625" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
-    <col min="8" max="8" width="25.5703125" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.59765625" customWidth="1"/>
+    <col min="9" max="9" width="17.86328125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.1328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.1328125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="18" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.3984375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -3201,7 +3600,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3209,7 +3608,7 @@
         <v>44691</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -3217,12 +3616,12 @@
         <v>267</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="D11" s="1" t="s">
         <v>5</v>
       </c>
@@ -3239,7 +3638,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="D12" s="5">
         <v>1</v>
       </c>
@@ -3250,7 +3649,7 @@
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D13" s="5">
         <v>2</v>
       </c>
@@ -3261,7 +3660,7 @@
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D14" s="5">
         <v>3</v>
       </c>
@@ -3272,7 +3671,7 @@
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="D15" s="5">
         <v>4</v>
       </c>
@@ -3283,7 +3682,7 @@
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="D16" s="5">
         <v>5</v>
       </c>
@@ -3294,105 +3693,105 @@
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
     </row>
-    <row r="18" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
     </row>
-    <row r="19" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
     </row>
-    <row r="20" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
     </row>
-    <row r="21" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
     </row>
-    <row r="22" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
     </row>
-    <row r="23" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
     </row>
-    <row r="24" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
     </row>
-    <row r="25" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
     </row>
-    <row r="26" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
     </row>
-    <row r="27" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
     </row>
-    <row r="28" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
     </row>
-    <row r="29" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
     </row>
-    <row r="30" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
     </row>
-    <row r="39" spans="4:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="4:15" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="D39" s="1" t="s">
         <v>10</v>
       </c>
@@ -3400,40 +3799,50 @@
         <v>11</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M39" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N39" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O39" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="P39" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="4:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="4:15" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="D40" t="s">
+        <v>310</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40" t="s">
+        <v>311</v>
+      </c>
+      <c r="I40" t="s">
+        <v>312</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="2">
@@ -3451,27 +3860,27 @@
       <selection activeCell="D54" sqref="D54:P54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.140625" customWidth="1"/>
-    <col min="3" max="3" width="28.5703125" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="75.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.1328125" customWidth="1"/>
+    <col min="3" max="3" width="28.59765625" customWidth="1"/>
+    <col min="4" max="4" width="20.59765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="75.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.86328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.1328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.3984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.86328125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.1328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.1328125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="18" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.3984375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -3482,7 +3891,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3490,7 +3899,7 @@
         <v>44691</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -3498,12 +3907,12 @@
         <v>267</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="D11" s="1" t="s">
         <v>5</v>
       </c>
@@ -3520,7 +3929,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="D12" s="5">
         <v>1</v>
       </c>
@@ -3531,7 +3940,7 @@
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D13" s="5">
         <v>2</v>
       </c>
@@ -3542,7 +3951,7 @@
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D14" s="5">
         <v>3</v>
       </c>
@@ -3553,7 +3962,7 @@
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D15" s="5">
         <v>4</v>
       </c>
@@ -3564,7 +3973,7 @@
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="D16" s="5">
         <v>5</v>
       </c>
@@ -3575,105 +3984,105 @@
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
     </row>
-    <row r="18" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
     </row>
-    <row r="19" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
     </row>
-    <row r="20" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
     </row>
-    <row r="21" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
     </row>
-    <row r="22" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
     </row>
-    <row r="23" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
     </row>
-    <row r="24" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
     </row>
-    <row r="25" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
     </row>
-    <row r="26" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
     </row>
-    <row r="27" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
     </row>
-    <row r="28" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
     </row>
-    <row r="29" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
     </row>
-    <row r="30" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
     </row>
-    <row r="39" spans="4:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="4:16" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="D39" s="1" t="s">
         <v>10</v>
       </c>
@@ -3714,7 +4123,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="4:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="4:16" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="2">
@@ -3732,26 +4141,26 @@
       <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="84.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="84.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="255.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="95.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="105.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="255.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="115.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.86328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="255.73046875" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="95.1328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.3984375" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="105.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="255.73046875" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="115.1328125" style="7" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="232" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="222.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="69.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="26.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="84.140625" style="7"/>
+    <col min="11" max="11" width="222.265625" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="69.1328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.73046875" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="84.1328125" style="7"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:11" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="3:11" ht="25.9" thickBot="1" x14ac:dyDescent="0.8">
       <c r="C3" s="6" t="s">
         <v>52</v>
       </c>
@@ -3771,7 +4180,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="3:11" ht="27" thickTop="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="3:11" ht="25.9" thickTop="1" x14ac:dyDescent="0.75">
       <c r="C4" s="6" t="s">
         <v>54</v>
       </c>
@@ -3791,7 +4200,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="3:11" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="5" spans="3:11" ht="25.5" x14ac:dyDescent="0.75">
       <c r="C5" s="6" t="s">
         <v>56</v>
       </c>
@@ -3811,7 +4220,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="3:11" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="6" spans="3:11" ht="25.5" x14ac:dyDescent="0.75">
       <c r="C6" s="6" t="s">
         <v>58</v>
       </c>
@@ -3831,7 +4240,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="3:11" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="7" spans="3:11" ht="25.5" x14ac:dyDescent="0.75">
       <c r="C7" s="6" t="s">
         <v>60</v>
       </c>
@@ -3851,7 +4260,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="3:11" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="8" spans="3:11" ht="25.5" x14ac:dyDescent="0.75">
       <c r="C8" s="6" t="s">
         <v>62</v>
       </c>
@@ -3871,7 +4280,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="9" spans="3:11" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="9" spans="3:11" ht="25.5" x14ac:dyDescent="0.75">
       <c r="C9" s="6" t="s">
         <v>64</v>
       </c>
@@ -3891,7 +4300,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="3:11" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="10" spans="3:11" ht="25.5" x14ac:dyDescent="0.75">
       <c r="C10" s="6" t="s">
         <v>66</v>
       </c>
@@ -3911,7 +4320,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="11" spans="3:11" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="11" spans="3:11" ht="25.5" x14ac:dyDescent="0.75">
       <c r="C11" s="6" t="s">
         <v>68</v>
       </c>
@@ -3931,7 +4340,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="12" spans="3:11" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="12" spans="3:11" ht="25.5" x14ac:dyDescent="0.75">
       <c r="C12" s="6" t="s">
         <v>70</v>
       </c>
@@ -3951,7 +4360,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="13" spans="3:11" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="13" spans="3:11" ht="25.5" x14ac:dyDescent="0.75">
       <c r="C13" s="6" t="s">
         <v>72</v>
       </c>
@@ -3971,7 +4380,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="14" spans="3:11" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="14" spans="3:11" ht="25.5" x14ac:dyDescent="0.75">
       <c r="C14" s="6" t="s">
         <v>74</v>
       </c>
@@ -3991,7 +4400,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="15" spans="3:11" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="15" spans="3:11" ht="25.5" x14ac:dyDescent="0.75">
       <c r="C15" s="6" t="s">
         <v>76</v>
       </c>
@@ -4011,7 +4420,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="16" spans="3:11" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="16" spans="3:11" ht="25.5" x14ac:dyDescent="0.75">
       <c r="C16" s="6" t="s">
         <v>78</v>
       </c>
@@ -4031,7 +4440,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="17" spans="3:11" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="17" spans="3:11" ht="25.5" x14ac:dyDescent="0.75">
       <c r="C17" s="6" t="s">
         <v>80</v>
       </c>
@@ -4051,7 +4460,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="18" spans="3:11" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="18" spans="3:11" ht="25.5" x14ac:dyDescent="0.75">
       <c r="C18" s="6" t="s">
         <v>82</v>
       </c>
@@ -4071,7 +4480,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="19" spans="3:11" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="19" spans="3:11" ht="25.5" x14ac:dyDescent="0.75">
       <c r="C19" s="6" t="s">
         <v>84</v>
       </c>
@@ -4091,7 +4500,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="20" spans="3:11" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="20" spans="3:11" ht="25.5" x14ac:dyDescent="0.75">
       <c r="C20" s="6" t="s">
         <v>86</v>
       </c>
@@ -4111,7 +4520,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="21" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:11" x14ac:dyDescent="0.45">
       <c r="H21" s="16">
         <v>18</v>
       </c>
@@ -4125,7 +4534,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="22" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:11" x14ac:dyDescent="0.45">
       <c r="H22" s="16">
         <v>19</v>
       </c>
@@ -4139,7 +4548,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="23" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:11" x14ac:dyDescent="0.45">
       <c r="H23" s="17">
         <v>20</v>
       </c>
@@ -4153,7 +4562,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="24" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:11" x14ac:dyDescent="0.45">
       <c r="H24" s="10">
         <v>21</v>
       </c>
@@ -4167,7 +4576,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="61" spans="1:14" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:14" ht="25.9" thickBot="1" x14ac:dyDescent="0.8">
       <c r="A61" s="19" t="s">
         <v>141</v>
       </c>
@@ -4211,7 +4620,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="62" spans="1:14" ht="19.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" ht="18.399999999999999" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A62" s="7" t="s">
         <v>143</v>
       </c>
@@ -4245,7 +4654,7 @@
       <c r="M62" s="24"/>
       <c r="N62" s="24"/>
     </row>
-    <row r="63" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" ht="18" x14ac:dyDescent="0.45">
       <c r="A63" s="7" t="s">
         <v>143</v>
       </c>
@@ -4279,7 +4688,7 @@
       <c r="M63" s="24"/>
       <c r="N63" s="24"/>
     </row>
-    <row r="64" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" ht="18" x14ac:dyDescent="0.45">
       <c r="A64" s="7" t="s">
         <v>154</v>
       </c>
@@ -4315,7 +4724,7 @@
       <c r="M64" s="24"/>
       <c r="N64" s="24"/>
     </row>
-    <row r="65" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" ht="18" x14ac:dyDescent="0.45">
       <c r="A65" s="7" t="s">
         <v>143</v>
       </c>
@@ -4349,7 +4758,7 @@
       <c r="M65" s="24"/>
       <c r="N65" s="24"/>
     </row>
-    <row r="66" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" ht="18" x14ac:dyDescent="0.45">
       <c r="A66" s="7" t="s">
         <v>143</v>
       </c>
@@ -4383,7 +4792,7 @@
       <c r="M66" s="24"/>
       <c r="N66" s="24"/>
     </row>
-    <row r="67" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" ht="18" x14ac:dyDescent="0.45">
       <c r="A67" s="7" t="s">
         <v>143</v>
       </c>
@@ -4417,7 +4826,7 @@
       <c r="M67" s="24"/>
       <c r="N67" s="24"/>
     </row>
-    <row r="68" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" ht="18" x14ac:dyDescent="0.45">
       <c r="A68" s="7" t="s">
         <v>143</v>
       </c>
@@ -4459,7 +4868,7 @@
       </c>
       <c r="N68" s="24"/>
     </row>
-    <row r="69" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" ht="18" x14ac:dyDescent="0.45">
       <c r="A69" s="7" t="s">
         <v>154</v>
       </c>
@@ -4501,7 +4910,7 @@
       </c>
       <c r="N69" s="24"/>
     </row>
-    <row r="70" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" ht="18" x14ac:dyDescent="0.45">
       <c r="A70" s="7" t="s">
         <v>186</v>
       </c>
@@ -4541,7 +4950,7 @@
       </c>
       <c r="N70" s="24"/>
     </row>
-    <row r="71" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" ht="18" x14ac:dyDescent="0.45">
       <c r="A71" s="7" t="s">
         <v>193</v>
       </c>
@@ -4583,7 +4992,7 @@
       </c>
       <c r="N71" s="24"/>
     </row>
-    <row r="72" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" ht="18" x14ac:dyDescent="0.45">
       <c r="A72" s="7" t="s">
         <v>186</v>
       </c>
@@ -4625,7 +5034,7 @@
       </c>
       <c r="N72" s="24"/>
     </row>
-    <row r="73" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" ht="18" x14ac:dyDescent="0.45">
       <c r="A73" s="7" t="s">
         <v>193</v>
       </c>
@@ -4667,7 +5076,7 @@
       </c>
       <c r="N73" s="24"/>
     </row>
-    <row r="74" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14" ht="18" x14ac:dyDescent="0.45">
       <c r="A74" s="7" t="s">
         <v>143</v>
       </c>
@@ -4701,7 +5110,7 @@
       <c r="M74" s="24"/>
       <c r="N74" s="24"/>
     </row>
-    <row r="75" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:14" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="7" t="s">
         <v>143</v>
       </c>
@@ -4733,7 +5142,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="76" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:14" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="7" t="s">
         <v>154</v>
       </c>
@@ -4771,7 +5180,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="77" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:14" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="7" t="s">
         <v>193</v>
       </c>
@@ -4797,7 +5206,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="78" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:14" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="7" t="s">
         <v>193</v>
       </c>
@@ -4823,7 +5232,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="79" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:14" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="7" t="s">
         <v>193</v>
       </c>
@@ -4858,7 +5267,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="80" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:14" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="7" t="s">
         <v>193</v>
       </c>
@@ -4887,7 +5296,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:10" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="7" t="s">
         <v>193</v>
       </c>
@@ -4916,7 +5325,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="82" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:10" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="7" t="s">
         <v>193</v>
       </c>
@@ -4942,7 +5351,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="83" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:10" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="30" t="s">
         <v>143</v>
       </c>
@@ -4968,7 +5377,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="84" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:10" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="7" t="s">
         <v>193</v>
       </c>
@@ -4997,7 +5406,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="85" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:10" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="7" t="s">
         <v>193</v>
       </c>
@@ -5026,7 +5435,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="86" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:10" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="30" t="s">
         <v>186</v>
       </c>
@@ -5052,7 +5461,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="87" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:10" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="7" t="s">
         <v>193</v>
       </c>

</xml_diff>